<commit_message>
Added Chicagod to Charlotte
</commit_message>
<xml_diff>
--- a/NFL_cities.xlsx
+++ b/NFL_cities.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="NFL City Mileages" sheetId="1" r:id="rId1"/>
@@ -615,16 +615,16 @@
   <dimension ref="A1:AI36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>72</v>
       </c>
@@ -731,7 +731,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>28</v>
       </c>
@@ -869,7 +869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -1006,7 +1006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
@@ -1139,7 +1139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
@@ -1268,7 +1268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="I6" s="3">
         <f>H7</f>
-        <v>0</v>
+        <v>754</v>
       </c>
       <c r="J6" s="3">
         <f>H8</f>
@@ -1393,7 +1393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -1403,6 +1403,9 @@
       <c r="C7" t="s">
         <v>71</v>
       </c>
+      <c r="H7">
+        <v>754</v>
+      </c>
       <c r="I7" s="4">
         <v>0</v>
       </c>
@@ -1511,7 +1514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>26</v>
       </c>
@@ -1625,7 +1628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>18</v>
       </c>
@@ -1741,7 +1744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
@@ -1847,7 +1850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
@@ -1949,7 +1952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>30</v>
       </c>
@@ -2047,7 +2050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
@@ -2141,7 +2144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -2231,7 +2234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -2317,7 +2320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>11</v>
       </c>
@@ -2399,7 +2402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
@@ -2477,7 +2480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>24</v>
       </c>
@@ -2551,7 +2554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>9</v>
       </c>
@@ -2621,7 +2624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>1</v>
       </c>
@@ -2687,7 +2690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>31</v>
       </c>
@@ -2749,7 +2752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>7</v>
       </c>
@@ -2807,7 +2810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>4</v>
       </c>
@@ -2861,7 +2864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>21</v>
       </c>
@@ -2911,7 +2914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>29</v>
       </c>
@@ -2957,7 +2960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>23</v>
       </c>
@@ -2999,7 +3002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>25</v>
       </c>
@@ -3040,7 +3043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>19</v>
       </c>
@@ -3074,7 +3077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>27</v>
       </c>
@@ -3104,7 +3107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>3</v>
       </c>
@@ -3130,7 +3133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>2</v>
       </c>
@@ -3152,7 +3155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>0</v>
       </c>
@@ -3170,7 +3173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>17</v>
       </c>
@@ -3184,7 +3187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
@@ -3221,7 +3224,7 @@
       <c r="AH34" s="5"/>
       <c r="AI34" s="5"/>
     </row>
-    <row r="36" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>73</v>
       </c>

</xml_diff>

<commit_message>
Finished mileage chart and added CSV
</commit_message>
<xml_diff>
--- a/NFL_cities.xlsx
+++ b/NFL_cities.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="78">
   <si>
     <t>TEN</t>
   </si>
@@ -237,17 +237,32 @@
     <t>NORTH</t>
   </si>
   <si>
+    <t>http://maps.randmcnally.com/mileage_calculator</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
     <t>Team</t>
   </si>
   <si>
-    <t>http://maps.randmcnally.com/mileage_calculator</t>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Median</t>
+  </si>
+  <si>
+    <t>Mode</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -266,6 +281,21 @@
     <font>
       <sz val="11"/>
       <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -318,10 +348,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -330,11 +362,20 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="9" fontId="1" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -612,10 +653,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI36"/>
+  <dimension ref="A1:AI40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -625,8 +669,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>72</v>
+      <c r="A1" s="6" t="s">
+        <v>74</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>64</v>
@@ -741,8 +785,8 @@
       <c r="C2" t="s">
         <v>68</v>
       </c>
-      <c r="D2" s="4">
-        <v>0</v>
+      <c r="D2" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="E2" s="3">
         <f>D3</f>
@@ -762,11 +806,11 @@
       </c>
       <c r="I2" s="3">
         <f>D7</f>
-        <v>0</v>
+        <v>1803</v>
       </c>
       <c r="J2" s="3">
         <f>D8</f>
-        <v>0</v>
+        <v>1867</v>
       </c>
       <c r="K2" s="3">
         <f>D9</f>
@@ -774,71 +818,71 @@
       </c>
       <c r="L2" s="3">
         <f>D10</f>
-        <v>0</v>
+        <v>1065</v>
       </c>
       <c r="M2" s="3">
         <f>D11</f>
-        <v>0</v>
+        <v>823</v>
       </c>
       <c r="N2" s="3">
         <f>D12</f>
-        <v>0</v>
+        <v>2031</v>
       </c>
       <c r="O2" s="3">
         <f>D13</f>
-        <v>0</v>
+        <v>1939</v>
       </c>
       <c r="P2" s="3">
         <f>D14</f>
-        <v>0</v>
+        <v>1177</v>
       </c>
       <c r="Q2" s="3">
         <f>D15</f>
-        <v>0</v>
+        <v>1750</v>
       </c>
       <c r="R2" s="3">
         <f>D16</f>
-        <v>0</v>
+        <v>2047</v>
       </c>
       <c r="S2" s="3">
         <f>D17</f>
-        <v>0</v>
+        <v>1360</v>
       </c>
       <c r="T2" s="3">
         <f>D18</f>
-        <v>0</v>
+        <v>2363</v>
       </c>
       <c r="U2" s="3">
         <f>D19</f>
-        <v>0</v>
+        <v>1796</v>
       </c>
       <c r="V2" s="3">
         <f>D20</f>
-        <v>0</v>
+        <v>2686</v>
       </c>
       <c r="W2" s="3">
         <f>D21</f>
-        <v>0</v>
+        <v>1523</v>
       </c>
       <c r="X2" s="3">
         <f>D22</f>
-        <v>0</v>
+        <v>2459</v>
       </c>
       <c r="Y2" s="3">
         <f>D23</f>
-        <v>0</v>
+        <v>2459</v>
       </c>
       <c r="Z2" s="3">
         <f>D24</f>
-        <v>0</v>
+        <v>742</v>
       </c>
       <c r="AA2" s="3">
         <f>D25</f>
-        <v>0</v>
+        <v>2394</v>
       </c>
       <c r="AB2" s="3">
         <f>D26</f>
-        <v>0</v>
+        <v>2110</v>
       </c>
       <c r="AC2" s="3">
         <f>D27</f>
@@ -846,27 +890,27 @@
       </c>
       <c r="AD2" s="3">
         <f>D28</f>
-        <v>0</v>
+        <v>1508</v>
       </c>
       <c r="AE2" s="3">
         <f>D29</f>
-        <v>0</v>
+        <v>754</v>
       </c>
       <c r="AF2" s="3">
         <f>D30</f>
-        <v>0</v>
+        <v>1509</v>
       </c>
       <c r="AG2" s="3">
         <f>D31</f>
-        <v>0</v>
+        <v>2158</v>
       </c>
       <c r="AH2" s="3">
         <f>D32</f>
-        <v>0</v>
+        <v>1682</v>
       </c>
       <c r="AI2" s="3">
         <f>D33</f>
-        <v>0</v>
+        <v>2348</v>
       </c>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.3">
@@ -882,128 +926,128 @@
       <c r="D3">
         <v>1856</v>
       </c>
-      <c r="E3" s="4">
-        <v>0</v>
+      <c r="E3" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="F3" s="3">
         <f>E4</f>
-        <v>0</v>
+        <v>677</v>
       </c>
       <c r="G3" s="3">
         <f>E5</f>
-        <v>0</v>
+        <v>894</v>
       </c>
       <c r="H3" s="3">
         <f>E6</f>
-        <v>0</v>
+        <v>244</v>
       </c>
       <c r="I3" s="3">
         <f>E7</f>
-        <v>0</v>
+        <v>709</v>
       </c>
       <c r="J3" s="3">
         <f>E8</f>
-        <v>0</v>
+        <v>461</v>
       </c>
       <c r="K3" s="3">
         <f>E9</f>
-        <v>0</v>
+        <v>710</v>
       </c>
       <c r="L3" s="3">
         <f>E10</f>
-        <v>0</v>
+        <v>782</v>
       </c>
       <c r="M3" s="3">
         <f>E11</f>
-        <v>0</v>
+        <v>1401</v>
       </c>
       <c r="N3" s="3">
         <f>E12</f>
-        <v>0</v>
+        <v>719</v>
       </c>
       <c r="O3" s="3">
         <f>E13</f>
-        <v>0</v>
+        <v>921</v>
       </c>
       <c r="P3" s="3">
         <f>E14</f>
-        <v>0</v>
+        <v>794</v>
       </c>
       <c r="Q3" s="3">
         <f>E15</f>
-        <v>0</v>
+        <v>528</v>
       </c>
       <c r="R3" s="3">
         <f>E16</f>
-        <v>0</v>
+        <v>346</v>
       </c>
       <c r="S3" s="3">
         <f>E17</f>
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="T3" s="3">
         <f>E18</f>
-        <v>0</v>
+        <v>662</v>
       </c>
       <c r="U3" s="3">
         <f>E19</f>
-        <v>0</v>
+        <v>1114</v>
       </c>
       <c r="V3" s="3">
         <f>E20</f>
-        <v>0</v>
+        <v>1095</v>
       </c>
       <c r="W3" s="3">
         <f>E21</f>
-        <v>0</v>
+        <v>469</v>
       </c>
       <c r="X3" s="3">
         <f>E22</f>
-        <v>0</v>
+        <v>881</v>
       </c>
       <c r="Y3" s="3">
         <f>E23</f>
-        <v>0</v>
+        <v>881</v>
       </c>
       <c r="Z3" s="3">
         <f>E24</f>
-        <v>0</v>
+        <v>2466</v>
       </c>
       <c r="AA3" s="3">
         <f>E25</f>
-        <v>0</v>
+        <v>774</v>
       </c>
       <c r="AB3" s="3">
         <f>E26</f>
-        <v>0</v>
+        <v>685</v>
       </c>
       <c r="AC3" s="3">
         <f>E27</f>
-        <v>0</v>
+        <v>2141</v>
       </c>
       <c r="AD3" s="3">
         <f>E28</f>
-        <v>0</v>
+        <v>2670</v>
       </c>
       <c r="AE3" s="3">
         <f>E29</f>
-        <v>0</v>
+        <v>2477</v>
       </c>
       <c r="AF3" s="3">
         <f>E30</f>
-        <v>0</v>
+        <v>553</v>
       </c>
       <c r="AG3" s="3">
         <f>E31</f>
-        <v>0</v>
+        <v>457</v>
       </c>
       <c r="AH3" s="3">
         <f>E32</f>
-        <v>0</v>
+        <v>248</v>
       </c>
       <c r="AI3" s="3">
         <f>E33</f>
-        <v>0</v>
+        <v>638</v>
       </c>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.3">
@@ -1019,124 +1063,127 @@
       <c r="D4">
         <v>2334</v>
       </c>
-      <c r="F4" s="4">
-        <v>0</v>
+      <c r="E4">
+        <v>677</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="G4" s="3">
         <f>F5</f>
-        <v>0</v>
+        <v>363</v>
       </c>
       <c r="H4" s="3">
         <f>F6</f>
-        <v>0</v>
+        <v>436</v>
       </c>
       <c r="I4" s="3">
         <f>F7</f>
-        <v>0</v>
+        <v>700</v>
       </c>
       <c r="J4" s="3">
         <f>F8</f>
-        <v>0</v>
+        <v>498</v>
       </c>
       <c r="K4" s="3">
         <f>F9</f>
-        <v>0</v>
+        <v>374</v>
       </c>
       <c r="L4" s="3">
         <f>F10</f>
-        <v>0</v>
+        <v>1364</v>
       </c>
       <c r="M4" s="3">
         <f>F11</f>
-        <v>0</v>
+        <v>1658</v>
       </c>
       <c r="N4" s="3">
         <f>F12</f>
-        <v>0</v>
+        <v>524</v>
       </c>
       <c r="O4" s="3">
         <f>F13</f>
-        <v>0</v>
+        <v>902</v>
       </c>
       <c r="P4" s="3">
         <f>F14</f>
-        <v>0</v>
+        <v>1450</v>
       </c>
       <c r="Q4" s="3">
         <f>F15</f>
-        <v>0</v>
+        <v>574</v>
       </c>
       <c r="R4" s="3">
         <f>F16</f>
-        <v>0</v>
+        <v>750</v>
       </c>
       <c r="S4" s="3">
         <f>F17</f>
-        <v>0</v>
+        <v>1057</v>
       </c>
       <c r="T4" s="3">
         <f>F18</f>
-        <v>0</v>
+        <v>1095</v>
       </c>
       <c r="U4" s="3">
         <f>F19</f>
-        <v>0</v>
+        <v>1109</v>
       </c>
       <c r="V4" s="3">
         <f>F20</f>
-        <v>0</v>
+        <v>401</v>
       </c>
       <c r="W4" s="3">
         <f>F21</f>
-        <v>0</v>
+        <v>1125</v>
       </c>
       <c r="X4" s="3">
         <f>F22</f>
-        <v>0</v>
+        <v>188</v>
       </c>
       <c r="Y4" s="3">
         <f>F23</f>
-        <v>0</v>
+        <v>188</v>
       </c>
       <c r="Z4" s="3">
         <f>F24</f>
-        <v>0</v>
+        <v>2813</v>
       </c>
       <c r="AA4" s="3">
         <f>F25</f>
-        <v>0</v>
+        <v>97</v>
       </c>
       <c r="AB4" s="3">
         <f>F26</f>
-        <v>0</v>
+        <v>246</v>
       </c>
       <c r="AC4" s="3">
         <f>F27</f>
-        <v>0</v>
+        <v>2667</v>
       </c>
       <c r="AD4" s="3">
         <f>F28</f>
-        <v>0</v>
+        <v>2800</v>
       </c>
       <c r="AE4" s="3">
         <f>F29</f>
-        <v>0</v>
+        <v>2819</v>
       </c>
       <c r="AF4" s="3">
         <f>F30</f>
-        <v>0</v>
+        <v>816</v>
       </c>
       <c r="AG4" s="3">
         <f>F31</f>
-        <v>0</v>
+        <v>947</v>
       </c>
       <c r="AH4" s="3">
         <f>F32</f>
-        <v>0</v>
+        <v>704</v>
       </c>
       <c r="AI4" s="3">
         <f>F33</f>
-        <v>0</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.3">
@@ -1152,120 +1199,126 @@
       <c r="D5">
         <v>2250</v>
       </c>
-      <c r="G5" s="4">
-        <v>0</v>
+      <c r="E5">
+        <v>894</v>
+      </c>
+      <c r="F5">
+        <v>363</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="H5" s="3">
         <f>G6</f>
-        <v>0</v>
+        <v>657</v>
       </c>
       <c r="I5" s="3">
         <f>G7</f>
-        <v>0</v>
+        <v>533</v>
       </c>
       <c r="J5" s="3">
         <f>G8</f>
-        <v>0</v>
+        <v>428</v>
       </c>
       <c r="K5" s="3">
         <f>G9</f>
-        <v>0</v>
+        <v>190</v>
       </c>
       <c r="L5" s="3">
         <f>G10</f>
-        <v>0</v>
+        <v>1364</v>
       </c>
       <c r="M5" s="3">
         <f>G11</f>
-        <v>0</v>
+        <v>1521</v>
       </c>
       <c r="N5" s="3">
         <f>G12</f>
-        <v>0</v>
+        <v>258</v>
       </c>
       <c r="O5" s="3">
         <f>G13</f>
-        <v>0</v>
+        <v>735</v>
       </c>
       <c r="P5" s="3">
         <f>G14</f>
-        <v>0</v>
+        <v>1559</v>
       </c>
       <c r="Q5" s="3">
         <f>G15</f>
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="R5" s="3">
         <f>G16</f>
-        <v>0</v>
+        <v>1038</v>
       </c>
       <c r="S5" s="3">
         <f>G17</f>
-        <v>0</v>
+        <v>983</v>
       </c>
       <c r="T5" s="3">
         <f>G18</f>
-        <v>0</v>
+        <v>1384</v>
       </c>
       <c r="U5" s="3">
         <f>G19</f>
-        <v>0</v>
+        <v>942</v>
       </c>
       <c r="V5" s="3">
         <f>G20</f>
-        <v>0</v>
+        <v>455</v>
       </c>
       <c r="W5" s="3">
         <f>G21</f>
-        <v>0</v>
+        <v>1237</v>
       </c>
       <c r="X5" s="3">
         <f>G22</f>
-        <v>0</v>
+        <v>379</v>
       </c>
       <c r="Y5" s="3">
         <f>G23</f>
-        <v>0</v>
+        <v>379</v>
       </c>
       <c r="Z5" s="3">
         <f>G24</f>
-        <v>0</v>
+        <v>2646</v>
       </c>
       <c r="AA5" s="3">
         <f>G25</f>
-        <v>0</v>
+        <v>381</v>
       </c>
       <c r="AB5" s="3">
         <f>G26</f>
-        <v>0</v>
+        <v>215</v>
       </c>
       <c r="AC5" s="3">
         <f>G27</f>
-        <v>0</v>
+        <v>2597</v>
       </c>
       <c r="AD5" s="3">
         <f>G28</f>
-        <v>0</v>
+        <v>2633</v>
       </c>
       <c r="AE5" s="3">
         <f>G29</f>
-        <v>0</v>
+        <v>2652</v>
       </c>
       <c r="AF5" s="3">
         <f>G30</f>
-        <v>0</v>
+        <v>742</v>
       </c>
       <c r="AG5" s="3">
         <f>G31</f>
-        <v>0</v>
+        <v>1235</v>
       </c>
       <c r="AH5" s="3">
         <f>G32</f>
-        <v>0</v>
+        <v>705</v>
       </c>
       <c r="AI5" s="3">
         <f>G33</f>
-        <v>0</v>
+        <v>382</v>
       </c>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.3">
@@ -1281,8 +1334,17 @@
       <c r="D6">
         <v>2090</v>
       </c>
-      <c r="H6" s="4">
-        <v>0</v>
+      <c r="E6">
+        <v>244</v>
+      </c>
+      <c r="F6">
+        <v>436</v>
+      </c>
+      <c r="G6">
+        <v>657</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="I6" s="3">
         <f>H7</f>
@@ -1290,107 +1352,107 @@
       </c>
       <c r="J6" s="3">
         <f>H8</f>
-        <v>0</v>
+        <v>482</v>
       </c>
       <c r="K6" s="3">
         <f>H9</f>
-        <v>0</v>
+        <v>517</v>
       </c>
       <c r="L6" s="3">
         <f>H10</f>
-        <v>0</v>
+        <v>1028</v>
       </c>
       <c r="M6" s="3">
         <f>H11</f>
-        <v>0</v>
+        <v>1562</v>
       </c>
       <c r="N6" s="3">
         <f>H12</f>
-        <v>0</v>
+        <v>668</v>
       </c>
       <c r="O6" s="3">
         <f>H13</f>
-        <v>0</v>
+        <v>965</v>
       </c>
       <c r="P6" s="3">
         <f>H14</f>
-        <v>0</v>
+        <v>1038</v>
       </c>
       <c r="Q6" s="3">
         <f>H15</f>
-        <v>0</v>
+        <v>575</v>
       </c>
       <c r="R6" s="3">
         <f>H16</f>
-        <v>0</v>
+        <v>384</v>
       </c>
       <c r="S6" s="3">
         <f>H17</f>
-        <v>0</v>
+        <v>961</v>
       </c>
       <c r="T6" s="3">
         <f>H18</f>
-        <v>0</v>
+        <v>730</v>
       </c>
       <c r="U6" s="3">
         <f>H19</f>
-        <v>0</v>
+        <v>1165</v>
       </c>
       <c r="V6" s="3">
         <f>H20</f>
-        <v>0</v>
+        <v>860</v>
       </c>
       <c r="W6" s="3">
         <f>H21</f>
-        <v>0</v>
+        <v>713</v>
       </c>
       <c r="X6" s="3">
         <f>H22</f>
-        <v>0</v>
+        <v>646</v>
       </c>
       <c r="Y6" s="3">
         <f>H23</f>
-        <v>0</v>
+        <v>646</v>
       </c>
       <c r="Z6" s="3">
         <f>H24</f>
-        <v>0</v>
+        <v>2762</v>
       </c>
       <c r="AA6" s="3">
         <f>H25</f>
-        <v>0</v>
+        <v>533</v>
       </c>
       <c r="AB6" s="3">
         <f>H26</f>
-        <v>0</v>
+        <v>450</v>
       </c>
       <c r="AC6" s="3">
         <f>H27</f>
-        <v>0</v>
+        <v>2387</v>
       </c>
       <c r="AD6" s="3">
         <f>H28</f>
-        <v>0</v>
+        <v>2831</v>
       </c>
       <c r="AE6" s="3">
         <f>H29</f>
-        <v>0</v>
+        <v>2768</v>
       </c>
       <c r="AF6" s="3">
         <f>H30</f>
-        <v>0</v>
+        <v>714</v>
       </c>
       <c r="AG6" s="3">
         <f>H31</f>
-        <v>0</v>
+        <v>581</v>
       </c>
       <c r="AH6" s="3">
         <f>H32</f>
-        <v>0</v>
+        <v>408</v>
       </c>
       <c r="AI6" s="3">
         <f>H33</f>
-        <v>0</v>
+        <v>397</v>
       </c>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.3">
@@ -1403,115 +1465,127 @@
       <c r="C7" t="s">
         <v>71</v>
       </c>
+      <c r="D7">
+        <v>1803</v>
+      </c>
+      <c r="E7">
+        <v>709</v>
+      </c>
+      <c r="F7">
+        <v>700</v>
+      </c>
+      <c r="G7">
+        <v>533</v>
+      </c>
       <c r="H7">
         <v>754</v>
       </c>
-      <c r="I7" s="4">
-        <v>0</v>
+      <c r="I7" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="J7" s="3">
         <f>I8</f>
-        <v>0</v>
+        <v>295</v>
       </c>
       <c r="K7" s="3">
         <f>I9</f>
-        <v>0</v>
+        <v>343</v>
       </c>
       <c r="L7" s="3">
         <f>I10</f>
-        <v>0</v>
+        <v>945</v>
       </c>
       <c r="M7" s="3">
         <f>I11</f>
-        <v>0</v>
+        <v>1004</v>
       </c>
       <c r="N7" s="3">
         <f>I12</f>
-        <v>0</v>
+        <v>286</v>
       </c>
       <c r="O7" s="3">
         <f>I13</f>
-        <v>0</v>
+        <v>203</v>
       </c>
       <c r="P7" s="3">
         <f>I14</f>
-        <v>0</v>
+        <v>1099</v>
       </c>
       <c r="Q7" s="3">
         <f>I15</f>
-        <v>0</v>
+        <v>184</v>
       </c>
       <c r="R7" s="3">
         <f>I16</f>
-        <v>0</v>
+        <v>1064</v>
       </c>
       <c r="S7" s="3">
         <f>I17</f>
-        <v>0</v>
+        <v>527</v>
       </c>
       <c r="T7" s="3">
         <f>I18</f>
-        <v>0</v>
+        <v>1380</v>
       </c>
       <c r="U7" s="3">
         <f>I19</f>
-        <v>0</v>
+        <v>410</v>
       </c>
       <c r="V7" s="3">
         <f>I20</f>
-        <v>0</v>
+        <v>990</v>
       </c>
       <c r="W7" s="3">
         <f>I21</f>
-        <v>0</v>
+        <v>925</v>
       </c>
       <c r="X7" s="3">
         <f>I22</f>
-        <v>0</v>
+        <v>789</v>
       </c>
       <c r="Y7" s="3">
         <f>I23</f>
-        <v>0</v>
+        <v>789</v>
       </c>
       <c r="Z7" s="3">
         <f>I24</f>
-        <v>0</v>
+        <v>2129</v>
       </c>
       <c r="AA7" s="3">
         <f>I25</f>
-        <v>0</v>
+        <v>758</v>
       </c>
       <c r="AB7" s="3">
         <f>I26</f>
-        <v>0</v>
+        <v>460</v>
       </c>
       <c r="AC7" s="3">
         <f>I27</f>
-        <v>0</v>
+        <v>2079</v>
       </c>
       <c r="AD7" s="3">
         <f>I28</f>
-        <v>0</v>
+        <v>2101</v>
       </c>
       <c r="AE7" s="3">
         <f>I29</f>
-        <v>0</v>
+        <v>2135</v>
       </c>
       <c r="AF7" s="3">
         <f>I30</f>
-        <v>0</v>
+        <v>294</v>
       </c>
       <c r="AG7" s="3">
         <f>I31</f>
-        <v>0</v>
+        <v>1175</v>
       </c>
       <c r="AH7" s="3">
         <f>I32</f>
-        <v>0</v>
+        <v>471</v>
       </c>
       <c r="AI7" s="3">
         <f>I33</f>
-        <v>0</v>
+        <v>696</v>
       </c>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.3">
@@ -1524,8 +1598,26 @@
       <c r="C8" t="s">
         <v>71</v>
       </c>
-      <c r="J8" s="4">
-        <v>0</v>
+      <c r="D8">
+        <v>1867</v>
+      </c>
+      <c r="E8">
+        <v>461</v>
+      </c>
+      <c r="F8">
+        <v>498</v>
+      </c>
+      <c r="G8">
+        <v>428</v>
+      </c>
+      <c r="H8">
+        <v>482</v>
+      </c>
+      <c r="I8">
+        <v>295</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="K8" s="3">
         <f>J9</f>
@@ -1533,99 +1625,99 @@
       </c>
       <c r="L8" s="3">
         <f>J10</f>
-        <v>0</v>
+        <v>938</v>
       </c>
       <c r="M8" s="3">
         <f>J11</f>
-        <v>0</v>
+        <v>1193</v>
       </c>
       <c r="N8" s="3">
         <f>J12</f>
-        <v>0</v>
+        <v>255</v>
       </c>
       <c r="O8" s="3">
         <f>J13</f>
-        <v>0</v>
+        <v>504</v>
       </c>
       <c r="P8" s="3">
         <f>J14</f>
-        <v>0</v>
+        <v>1133</v>
       </c>
       <c r="Q8" s="3">
         <f>J15</f>
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="R8" s="3">
         <f>J16</f>
-        <v>0</v>
+        <v>803</v>
       </c>
       <c r="S8" s="3">
         <f>J17</f>
-        <v>0</v>
+        <v>591</v>
       </c>
       <c r="T8" s="3">
         <f>J18</f>
-        <v>0</v>
+        <v>1130</v>
       </c>
       <c r="U8" s="3">
         <f>J19</f>
-        <v>0</v>
+        <v>703</v>
       </c>
       <c r="V8" s="3">
         <f>J20</f>
-        <v>0</v>
+        <v>864</v>
       </c>
       <c r="W8" s="3">
         <f>J21</f>
-        <v>0</v>
+        <v>811</v>
       </c>
       <c r="X8" s="3">
         <f>J22</f>
-        <v>0</v>
+        <v>633</v>
       </c>
       <c r="Y8" s="3">
         <f>J23</f>
-        <v>0</v>
+        <v>633</v>
       </c>
       <c r="Z8" s="3">
         <f>J24</f>
-        <v>0</v>
+        <v>2382</v>
       </c>
       <c r="AA8" s="3">
         <f>J25</f>
-        <v>0</v>
+        <v>568</v>
       </c>
       <c r="AB8" s="3">
         <f>J26</f>
-        <v>0</v>
+        <v>284</v>
       </c>
       <c r="AC8" s="3">
         <f>J27</f>
-        <v>0</v>
+        <v>2202</v>
       </c>
       <c r="AD8" s="3">
         <f>J28</f>
-        <v>0</v>
+        <v>2388</v>
       </c>
       <c r="AE8" s="3">
         <f>J29</f>
-        <v>0</v>
+        <v>2388</v>
       </c>
       <c r="AF8" s="3">
         <f>J30</f>
-        <v>0</v>
+        <v>351</v>
       </c>
       <c r="AG8" s="3">
         <f>J31</f>
-        <v>0</v>
+        <v>925</v>
       </c>
       <c r="AH8" s="3">
         <f>J32</f>
-        <v>0</v>
+        <v>279</v>
       </c>
       <c r="AI8" s="3">
         <f>J33</f>
-        <v>0</v>
+        <v>506</v>
       </c>
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.3">
@@ -1641,107 +1733,122 @@
       <c r="D9">
         <v>2066</v>
       </c>
+      <c r="E9">
+        <v>710</v>
+      </c>
+      <c r="F9">
+        <v>374</v>
+      </c>
+      <c r="G9">
+        <v>190</v>
+      </c>
+      <c r="H9">
+        <v>517</v>
+      </c>
+      <c r="I9">
+        <v>343</v>
+      </c>
       <c r="J9">
         <v>244</v>
       </c>
-      <c r="K9" s="4">
-        <v>0</v>
+      <c r="K9" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="L9" s="3">
         <f>K10</f>
-        <v>0</v>
+        <v>1180</v>
       </c>
       <c r="M9" s="3">
         <f>K11</f>
-        <v>0</v>
+        <v>1332</v>
       </c>
       <c r="N9" s="3">
         <f>K12</f>
-        <v>0</v>
+        <v>168</v>
       </c>
       <c r="O9" s="3">
         <f>K13</f>
-        <v>0</v>
+        <v>546</v>
       </c>
       <c r="P9" s="3">
         <f>K14</f>
-        <v>0</v>
+        <v>1376</v>
       </c>
       <c r="Q9" s="3">
         <f>K15</f>
-        <v>0</v>
+        <v>317</v>
       </c>
       <c r="R9" s="3">
         <f>K16</f>
-        <v>0</v>
+        <v>898</v>
       </c>
       <c r="S9" s="3">
         <f>K17</f>
-        <v>0</v>
+        <v>799</v>
       </c>
       <c r="T9" s="3">
         <f>K18</f>
-        <v>0</v>
+        <v>1243</v>
       </c>
       <c r="U9" s="3">
         <f>K19</f>
-        <v>0</v>
+        <v>753</v>
       </c>
       <c r="V9" s="3">
         <f>K20</f>
-        <v>0</v>
+        <v>639</v>
       </c>
       <c r="W9" s="3">
         <f>K21</f>
-        <v>0</v>
+        <v>1053</v>
       </c>
       <c r="X9" s="3">
         <f>K22</f>
-        <v>0</v>
+        <v>464</v>
       </c>
       <c r="Y9" s="3">
         <f>K23</f>
-        <v>0</v>
+        <v>464</v>
       </c>
       <c r="Z9" s="3">
         <f>K24</f>
-        <v>0</v>
+        <v>2457</v>
       </c>
       <c r="AA9" s="3">
         <f>K25</f>
-        <v>0</v>
+        <v>433</v>
       </c>
       <c r="AB9" s="3">
         <f>K26</f>
-        <v>0</v>
+        <v>134</v>
       </c>
       <c r="AC9" s="3">
         <f>K27</f>
-        <v>0</v>
+        <v>2408</v>
       </c>
       <c r="AD9" s="3">
         <f>K28</f>
-        <v>0</v>
+        <v>2444</v>
       </c>
       <c r="AE9" s="3">
         <f>K29</f>
-        <v>0</v>
+        <v>2463</v>
       </c>
       <c r="AF9" s="3">
         <f>K30</f>
-        <v>0</v>
+        <v>559</v>
       </c>
       <c r="AG9" s="3">
         <f>K31</f>
-        <v>0</v>
+        <v>1095</v>
       </c>
       <c r="AH9" s="3">
         <f>K32</f>
-        <v>0</v>
+        <v>521</v>
       </c>
       <c r="AI9" s="3">
         <f>K33</f>
-        <v>0</v>
+        <v>371</v>
       </c>
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.3">
@@ -1754,100 +1861,124 @@
       <c r="C10" t="s">
         <v>70</v>
       </c>
-      <c r="L10" s="4">
-        <v>0</v>
+      <c r="D10">
+        <v>1065</v>
+      </c>
+      <c r="E10">
+        <v>782</v>
+      </c>
+      <c r="F10">
+        <v>1364</v>
+      </c>
+      <c r="G10">
+        <v>1364</v>
+      </c>
+      <c r="H10">
+        <v>1028</v>
+      </c>
+      <c r="I10">
+        <v>945</v>
+      </c>
+      <c r="J10">
+        <v>938</v>
+      </c>
+      <c r="K10">
+        <v>1180</v>
+      </c>
+      <c r="L10" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="M10" s="3">
         <f>L11</f>
-        <v>0</v>
+        <v>880</v>
       </c>
       <c r="N10" s="3">
         <f>L12</f>
-        <v>0</v>
+        <v>1181</v>
       </c>
       <c r="O10" s="3">
         <f>L13</f>
-        <v>0</v>
+        <v>1137</v>
       </c>
       <c r="P10" s="3">
         <f>L14</f>
-        <v>0</v>
+        <v>239</v>
       </c>
       <c r="Q10" s="3">
         <f>L15</f>
-        <v>0</v>
+        <v>900</v>
       </c>
       <c r="R10" s="3">
         <f>L16</f>
-        <v>0</v>
+        <v>1029</v>
       </c>
       <c r="S10" s="3">
         <f>L17</f>
-        <v>0</v>
+        <v>555</v>
       </c>
       <c r="T10" s="3">
         <f>L18</f>
-        <v>0</v>
+        <v>1345</v>
       </c>
       <c r="U10" s="3">
         <f>L19</f>
-        <v>0</v>
+        <v>991</v>
       </c>
       <c r="V10" s="3">
         <f>L20</f>
-        <v>0</v>
+        <v>1761</v>
       </c>
       <c r="W10" s="3">
         <f>L21</f>
-        <v>0</v>
+        <v>505</v>
       </c>
       <c r="X10" s="3">
         <f>L22</f>
-        <v>0</v>
+        <v>1546</v>
       </c>
       <c r="Y10" s="3">
         <f>L23</f>
-        <v>0</v>
+        <v>1546</v>
       </c>
       <c r="Z10" s="3">
         <f>L24</f>
-        <v>0</v>
+        <v>1824</v>
       </c>
       <c r="AA10" s="3">
         <f>L25</f>
-        <v>0</v>
+        <v>1462</v>
       </c>
       <c r="AB10" s="3">
         <f>L26</f>
-        <v>0</v>
+        <v>1220</v>
       </c>
       <c r="AC10" s="3">
         <f>L27</f>
-        <v>0</v>
+        <v>1360</v>
       </c>
       <c r="AD10" s="3">
         <f>L28</f>
-        <v>0</v>
+        <v>2204</v>
       </c>
       <c r="AE10" s="3">
         <f>L29</f>
-        <v>0</v>
+        <v>1835</v>
       </c>
       <c r="AF10" s="3">
         <f>L30</f>
-        <v>0</v>
+        <v>652</v>
       </c>
       <c r="AG10" s="3">
         <f>L31</f>
-        <v>0</v>
+        <v>1140</v>
       </c>
       <c r="AH10" s="3">
         <f>L32</f>
-        <v>0</v>
+        <v>661</v>
       </c>
       <c r="AI10" s="3">
         <f>L33</f>
-        <v>0</v>
+        <v>1327</v>
       </c>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.3">
@@ -1860,96 +1991,123 @@
       <c r="C11" t="s">
         <v>68</v>
       </c>
-      <c r="M11" s="4">
-        <v>0</v>
+      <c r="D11">
+        <v>823</v>
+      </c>
+      <c r="E11">
+        <v>1401</v>
+      </c>
+      <c r="F11">
+        <v>1658</v>
+      </c>
+      <c r="G11">
+        <v>1521</v>
+      </c>
+      <c r="H11">
+        <v>1562</v>
+      </c>
+      <c r="I11">
+        <v>1004</v>
+      </c>
+      <c r="J11">
+        <v>1193</v>
+      </c>
+      <c r="K11">
+        <v>1332</v>
+      </c>
+      <c r="L11">
+        <v>880</v>
+      </c>
+      <c r="M11" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="N11" s="3">
         <f>M12</f>
-        <v>0</v>
+        <v>1270</v>
       </c>
       <c r="O11" s="3">
         <f>M13</f>
-        <v>0</v>
+        <v>1102</v>
       </c>
       <c r="P11" s="3">
         <f>M14</f>
-        <v>0</v>
+        <v>1120</v>
       </c>
       <c r="Q11" s="3">
         <f>M15</f>
-        <v>0</v>
+        <v>1086</v>
       </c>
       <c r="R11" s="3">
         <f>M16</f>
-        <v>0</v>
+        <v>1751</v>
       </c>
       <c r="S11" s="3">
         <f>M17</f>
-        <v>0</v>
+        <v>603</v>
       </c>
       <c r="T11" s="3">
         <f>M18</f>
-        <v>0</v>
+        <v>2068</v>
       </c>
       <c r="U11" s="3">
         <f>M19</f>
-        <v>0</v>
+        <v>914</v>
       </c>
       <c r="V11" s="3">
         <f>M20</f>
-        <v>0</v>
+        <v>1981</v>
       </c>
       <c r="W11" s="3">
         <f>M21</f>
-        <v>0</v>
+        <v>1383</v>
       </c>
       <c r="X11" s="3">
         <f>M22</f>
-        <v>0</v>
+        <v>1780</v>
       </c>
       <c r="Y11" s="3">
         <f>M23</f>
-        <v>0</v>
+        <v>1780</v>
       </c>
       <c r="Z11" s="3">
         <f>M24</f>
-        <v>0</v>
+        <v>1263</v>
       </c>
       <c r="AA11" s="3">
         <f>M25</f>
-        <v>0</v>
+        <v>1729</v>
       </c>
       <c r="AB11" s="3">
         <f>M26</f>
-        <v>0</v>
+        <v>1445</v>
       </c>
       <c r="AC11" s="3">
         <f>M27</f>
-        <v>0</v>
+        <v>1079</v>
       </c>
       <c r="AD11" s="3">
         <f>M28</f>
-        <v>0</v>
+        <v>1332</v>
       </c>
       <c r="AE11" s="3">
         <f>M29</f>
-        <v>0</v>
+        <v>1269</v>
       </c>
       <c r="AF11" s="3">
         <f>M30</f>
-        <v>0</v>
+        <v>851</v>
       </c>
       <c r="AG11" s="3">
         <f>M31</f>
-        <v>0</v>
+        <v>1861</v>
       </c>
       <c r="AH11" s="3">
         <f>M32</f>
-        <v>0</v>
+        <v>1158</v>
       </c>
       <c r="AI11" s="3">
         <f>M33</f>
-        <v>0</v>
+        <v>1667</v>
       </c>
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.3">
@@ -1962,92 +2120,122 @@
       <c r="C12" t="s">
         <v>71</v>
       </c>
-      <c r="N12" s="4">
-        <v>0</v>
+      <c r="D12">
+        <v>2031</v>
+      </c>
+      <c r="E12">
+        <v>719</v>
+      </c>
+      <c r="F12">
+        <v>524</v>
+      </c>
+      <c r="G12">
+        <v>258</v>
+      </c>
+      <c r="H12">
+        <v>668</v>
+      </c>
+      <c r="I12">
+        <v>286</v>
+      </c>
+      <c r="J12">
+        <v>255</v>
+      </c>
+      <c r="K12">
+        <v>168</v>
+      </c>
+      <c r="L12">
+        <v>1181</v>
+      </c>
+      <c r="M12">
+        <v>1270</v>
+      </c>
+      <c r="N12" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="O12" s="3">
         <f>N13</f>
-        <v>0</v>
+        <v>484</v>
       </c>
       <c r="P12" s="3">
         <f>N14</f>
-        <v>0</v>
+        <v>1315</v>
       </c>
       <c r="Q12" s="3">
         <f>N15</f>
-        <v>0</v>
+        <v>277</v>
       </c>
       <c r="R12" s="3">
         <f>N16</f>
-        <v>0</v>
+        <v>1011</v>
       </c>
       <c r="S12" s="3">
         <f>N17</f>
-        <v>0</v>
+        <v>792</v>
       </c>
       <c r="T12" s="3">
         <f>N18</f>
-        <v>0</v>
+        <v>1357</v>
       </c>
       <c r="U12" s="3">
         <f>N19</f>
-        <v>0</v>
+        <v>694</v>
       </c>
       <c r="V12" s="3">
         <f>N20</f>
-        <v>0</v>
+        <v>706</v>
       </c>
       <c r="W12" s="3">
         <f>N21</f>
-        <v>0</v>
+        <v>1066</v>
       </c>
       <c r="X12" s="3">
         <f>N22</f>
-        <v>0</v>
+        <v>615</v>
       </c>
       <c r="Y12" s="3">
         <f>N23</f>
-        <v>0</v>
+        <v>615</v>
       </c>
       <c r="Z12" s="3">
         <f>N24</f>
-        <v>0</v>
+        <v>2394</v>
       </c>
       <c r="AA12" s="3">
         <f>N25</f>
-        <v>0</v>
+        <v>584</v>
       </c>
       <c r="AB12" s="3">
         <f>N26</f>
-        <v>0</v>
+        <v>285</v>
       </c>
       <c r="AC12" s="3">
         <f>N27</f>
-        <v>0</v>
+        <v>2344</v>
       </c>
       <c r="AD12" s="3">
         <f>N28</f>
-        <v>0</v>
+        <v>2386</v>
       </c>
       <c r="AE12" s="3">
         <f>N29</f>
-        <v>0</v>
+        <v>2400</v>
       </c>
       <c r="AF12" s="3">
         <f>N30</f>
-        <v>0</v>
+        <v>525</v>
       </c>
       <c r="AG12" s="3">
         <f>N31</f>
-        <v>0</v>
+        <v>1179</v>
       </c>
       <c r="AH12" s="3">
         <f>N32</f>
-        <v>0</v>
+        <v>534</v>
       </c>
       <c r="AI12" s="3">
         <f>N33</f>
-        <v>0</v>
+        <v>522</v>
       </c>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.3">
@@ -2060,88 +2248,121 @@
       <c r="C13" t="s">
         <v>71</v>
       </c>
-      <c r="O13" s="4">
-        <v>0</v>
+      <c r="D13">
+        <v>1939</v>
+      </c>
+      <c r="E13">
+        <v>921</v>
+      </c>
+      <c r="F13">
+        <v>902</v>
+      </c>
+      <c r="G13">
+        <v>735</v>
+      </c>
+      <c r="H13">
+        <v>965</v>
+      </c>
+      <c r="I13">
+        <v>203</v>
+      </c>
+      <c r="J13">
+        <v>504</v>
+      </c>
+      <c r="K13">
+        <v>546</v>
+      </c>
+      <c r="L13">
+        <v>1137</v>
+      </c>
+      <c r="M13">
+        <v>1102</v>
+      </c>
+      <c r="N13">
+        <v>484</v>
+      </c>
+      <c r="O13" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="P13" s="3">
         <f>O14</f>
-        <v>0</v>
+        <v>1304</v>
       </c>
       <c r="Q13" s="3">
         <f>O15</f>
-        <v>0</v>
+        <v>394</v>
       </c>
       <c r="R13" s="3">
         <f>O16</f>
-        <v>0</v>
+        <v>1275</v>
       </c>
       <c r="S13" s="3">
         <f>O17</f>
-        <v>0</v>
+        <v>626</v>
       </c>
       <c r="T13" s="3">
         <f>O18</f>
-        <v>0</v>
+        <v>1591</v>
       </c>
       <c r="U13" s="3">
         <f>O19</f>
-        <v>0</v>
+        <v>279</v>
       </c>
       <c r="V13" s="3">
         <f>O20</f>
-        <v>0</v>
+        <v>1197</v>
       </c>
       <c r="W13" s="3">
         <f>O21</f>
-        <v>0</v>
+        <v>1130</v>
       </c>
       <c r="X13" s="3">
         <f>O22</f>
-        <v>0</v>
+        <v>996</v>
       </c>
       <c r="Y13" s="3">
         <f>O23</f>
-        <v>0</v>
+        <v>996</v>
       </c>
       <c r="Z13" s="3">
         <f>O24</f>
-        <v>0</v>
+        <v>2227</v>
       </c>
       <c r="AA13" s="3">
         <f>O25</f>
-        <v>0</v>
+        <v>965</v>
       </c>
       <c r="AB13" s="3">
         <f>O26</f>
-        <v>0</v>
+        <v>666</v>
       </c>
       <c r="AC13" s="3">
         <f>O27</f>
-        <v>0</v>
+        <v>2178</v>
       </c>
       <c r="AD13" s="3">
         <f>O28</f>
-        <v>0</v>
+        <v>1937</v>
       </c>
       <c r="AE13" s="3">
         <f>O29</f>
-        <v>0</v>
+        <v>2233</v>
       </c>
       <c r="AF13" s="3">
         <f>O30</f>
-        <v>0</v>
+        <v>487</v>
       </c>
       <c r="AG13" s="3">
         <f>O31</f>
-        <v>0</v>
+        <v>1386</v>
       </c>
       <c r="AH13" s="3">
         <f>O32</f>
-        <v>0</v>
+        <v>681</v>
       </c>
       <c r="AI13" s="3">
         <f>O33</f>
-        <v>0</v>
+        <v>903</v>
       </c>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.3">
@@ -2154,84 +2375,120 @@
       <c r="C14" t="s">
         <v>69</v>
       </c>
-      <c r="P14" s="4">
-        <v>0</v>
+      <c r="D14">
+        <v>1177</v>
+      </c>
+      <c r="E14">
+        <v>794</v>
+      </c>
+      <c r="F14">
+        <v>1450</v>
+      </c>
+      <c r="G14">
+        <v>1559</v>
+      </c>
+      <c r="H14">
+        <v>1038</v>
+      </c>
+      <c r="I14">
+        <v>1099</v>
+      </c>
+      <c r="J14">
+        <v>1133</v>
+      </c>
+      <c r="K14">
+        <v>1376</v>
+      </c>
+      <c r="L14">
+        <v>239</v>
+      </c>
+      <c r="M14">
+        <v>1120</v>
+      </c>
+      <c r="N14">
+        <v>1315</v>
+      </c>
+      <c r="O14">
+        <v>1304</v>
+      </c>
+      <c r="P14" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="Q14" s="3">
         <f>P15</f>
-        <v>0</v>
+        <v>1033</v>
       </c>
       <c r="R14" s="3">
         <f>P16</f>
-        <v>0</v>
+        <v>872</v>
       </c>
       <c r="S14" s="3">
         <f>P17</f>
-        <v>0</v>
+        <v>794</v>
       </c>
       <c r="T14" s="3">
         <f>P18</f>
-        <v>0</v>
+        <v>1188</v>
       </c>
       <c r="U14" s="3">
         <f>P19</f>
-        <v>0</v>
+        <v>1230</v>
       </c>
       <c r="V14" s="3">
         <f>P20</f>
-        <v>0</v>
+        <v>1845</v>
       </c>
       <c r="W14" s="3">
         <f>P21</f>
-        <v>0</v>
+        <v>348</v>
       </c>
       <c r="X14" s="3">
         <f>P22</f>
-        <v>0</v>
+        <v>1631</v>
       </c>
       <c r="Y14" s="3">
         <f>P23</f>
-        <v>0</v>
+        <v>1631</v>
       </c>
       <c r="Z14" s="3">
         <f>P24</f>
-        <v>0</v>
+        <v>1918</v>
       </c>
       <c r="AA14" s="3">
         <f>P25</f>
-        <v>0</v>
+        <v>1547</v>
       </c>
       <c r="AB14" s="3">
         <f>P26</f>
-        <v>0</v>
+        <v>1418</v>
       </c>
       <c r="AC14" s="3">
         <f>P27</f>
-        <v>0</v>
+        <v>1472</v>
       </c>
       <c r="AD14" s="3">
         <f>P28</f>
-        <v>0</v>
+        <v>2443</v>
       </c>
       <c r="AE14" s="3">
         <f>P29</f>
-        <v>0</v>
+        <v>1930</v>
       </c>
       <c r="AF14" s="3">
         <f>P30</f>
-        <v>0</v>
+        <v>851</v>
       </c>
       <c r="AG14" s="3">
         <f>P31</f>
-        <v>0</v>
+        <v>983</v>
       </c>
       <c r="AH14" s="3">
         <f>P32</f>
-        <v>0</v>
+        <v>857</v>
       </c>
       <c r="AI14" s="3">
         <f>P33</f>
-        <v>0</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.3">
@@ -2244,80 +2501,119 @@
       <c r="C15" t="s">
         <v>69</v>
       </c>
-      <c r="Q15" s="4">
-        <v>0</v>
+      <c r="D15">
+        <v>1750</v>
+      </c>
+      <c r="E15">
+        <v>528</v>
+      </c>
+      <c r="F15">
+        <v>574</v>
+      </c>
+      <c r="G15">
+        <v>500</v>
+      </c>
+      <c r="H15">
+        <v>575</v>
+      </c>
+      <c r="I15">
+        <v>184</v>
+      </c>
+      <c r="J15">
+        <v>110</v>
+      </c>
+      <c r="K15">
+        <v>317</v>
+      </c>
+      <c r="L15">
+        <v>900</v>
+      </c>
+      <c r="M15">
+        <v>1086</v>
+      </c>
+      <c r="N15">
+        <v>277</v>
+      </c>
+      <c r="O15">
+        <v>394</v>
+      </c>
+      <c r="P15">
+        <v>1033</v>
+      </c>
+      <c r="Q15" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="R15" s="3">
         <f>Q16</f>
-        <v>0</v>
+        <v>881</v>
       </c>
       <c r="S15" s="3">
         <f>Q17</f>
-        <v>0</v>
+        <v>483</v>
       </c>
       <c r="T15" s="3">
         <f>Q18</f>
-        <v>0</v>
+        <v>1197</v>
       </c>
       <c r="U15" s="3">
         <f>Q19</f>
-        <v>0</v>
+        <v>592</v>
       </c>
       <c r="V15" s="3">
         <f>Q20</f>
-        <v>0</v>
+        <v>936</v>
       </c>
       <c r="W15" s="3">
         <f>Q21</f>
-        <v>0</v>
+        <v>820</v>
       </c>
       <c r="X15" s="3">
         <f>Q22</f>
-        <v>0</v>
+        <v>709</v>
       </c>
       <c r="Y15" s="3">
         <f>Q23</f>
-        <v>0</v>
+        <v>709</v>
       </c>
       <c r="Z15" s="3">
         <f>Q24</f>
-        <v>0</v>
+        <v>2268</v>
       </c>
       <c r="AA15" s="3">
         <f>Q25</f>
-        <v>0</v>
+        <v>644</v>
       </c>
       <c r="AB15" s="3">
         <f>Q26</f>
-        <v>0</v>
+        <v>360</v>
       </c>
       <c r="AC15" s="3">
         <f>Q27</f>
-        <v>0</v>
+        <v>2093</v>
       </c>
       <c r="AD15" s="3">
         <f>Q28</f>
-        <v>0</v>
+        <v>2273</v>
       </c>
       <c r="AE15" s="3">
         <f>Q29</f>
-        <v>0</v>
+        <v>2274</v>
       </c>
       <c r="AF15" s="3">
         <f>Q30</f>
-        <v>0</v>
+        <v>242</v>
       </c>
       <c r="AG15" s="3">
         <f>Q31</f>
-        <v>0</v>
+        <v>992</v>
       </c>
       <c r="AH15" s="3">
         <f>Q32</f>
-        <v>0</v>
+        <v>287</v>
       </c>
       <c r="AI15" s="3">
         <f>Q33</f>
-        <v>0</v>
+        <v>582</v>
       </c>
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.3">
@@ -2330,76 +2626,118 @@
       <c r="C16" t="s">
         <v>69</v>
       </c>
-      <c r="R16" s="4">
-        <v>0</v>
+      <c r="D16">
+        <v>2047</v>
+      </c>
+      <c r="E16">
+        <v>346</v>
+      </c>
+      <c r="F16">
+        <v>750</v>
+      </c>
+      <c r="G16">
+        <v>1038</v>
+      </c>
+      <c r="H16">
+        <v>384</v>
+      </c>
+      <c r="I16">
+        <v>1064</v>
+      </c>
+      <c r="J16">
+        <v>803</v>
+      </c>
+      <c r="K16">
+        <v>898</v>
+      </c>
+      <c r="L16">
+        <v>1029</v>
+      </c>
+      <c r="M16">
+        <v>1751</v>
+      </c>
+      <c r="N16">
+        <v>1011</v>
+      </c>
+      <c r="O16">
+        <v>1275</v>
+      </c>
+      <c r="P16">
+        <v>872</v>
+      </c>
+      <c r="Q16">
+        <v>881</v>
+      </c>
+      <c r="R16" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="S16" s="3">
         <f>R17</f>
-        <v>0</v>
+        <v>1146</v>
       </c>
       <c r="T16" s="3">
         <f>R18</f>
-        <v>0</v>
+        <v>346</v>
       </c>
       <c r="U16" s="3">
         <f>R19</f>
-        <v>0</v>
+        <v>1460</v>
       </c>
       <c r="V16" s="3">
         <f>R20</f>
-        <v>0</v>
+        <v>1150</v>
       </c>
       <c r="W16" s="3">
         <f>R21</f>
-        <v>0</v>
+        <v>547</v>
       </c>
       <c r="X16" s="3">
         <f>R22</f>
-        <v>0</v>
+        <v>938</v>
       </c>
       <c r="Y16" s="3">
         <f>R23</f>
-        <v>0</v>
+        <v>938</v>
       </c>
       <c r="Z16" s="3">
         <f>R24</f>
-        <v>0</v>
+        <v>2812</v>
       </c>
       <c r="AA16" s="3">
         <f>R25</f>
-        <v>0</v>
+        <v>847</v>
       </c>
       <c r="AB16" s="3">
         <f>R26</f>
-        <v>0</v>
+        <v>831</v>
       </c>
       <c r="AC16" s="3">
         <f>R27</f>
-        <v>0</v>
+        <v>2341</v>
       </c>
       <c r="AD16" s="3">
         <f>R28</f>
-        <v>0</v>
+        <v>3016</v>
       </c>
       <c r="AE16" s="3">
         <f>R29</f>
-        <v>0</v>
+        <v>2823</v>
       </c>
       <c r="AF16" s="3">
         <f>R30</f>
-        <v>0</v>
+        <v>899</v>
       </c>
       <c r="AG16" s="3">
         <f>R31</f>
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="AH16" s="3">
         <f>R32</f>
-        <v>0</v>
+        <v>593</v>
       </c>
       <c r="AI16" s="3">
         <f>R33</f>
-        <v>0</v>
+        <v>711</v>
       </c>
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.3">
@@ -2412,72 +2750,117 @@
       <c r="C17" t="s">
         <v>68</v>
       </c>
-      <c r="S17" s="4">
-        <v>0</v>
+      <c r="D17">
+        <v>1360</v>
+      </c>
+      <c r="E17">
+        <v>800</v>
+      </c>
+      <c r="F17">
+        <v>1057</v>
+      </c>
+      <c r="G17">
+        <v>983</v>
+      </c>
+      <c r="H17">
+        <v>961</v>
+      </c>
+      <c r="I17">
+        <v>527</v>
+      </c>
+      <c r="J17">
+        <v>591</v>
+      </c>
+      <c r="K17">
+        <v>799</v>
+      </c>
+      <c r="L17">
+        <v>555</v>
+      </c>
+      <c r="M17">
+        <v>603</v>
+      </c>
+      <c r="N17">
+        <v>792</v>
+      </c>
+      <c r="O17">
+        <v>626</v>
+      </c>
+      <c r="P17">
+        <v>794</v>
+      </c>
+      <c r="Q17">
+        <v>483</v>
+      </c>
+      <c r="R17">
+        <v>1146</v>
+      </c>
+      <c r="S17" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="T17" s="3">
         <f>S18</f>
-        <v>0</v>
+        <v>1464</v>
       </c>
       <c r="U17" s="3">
         <f>S19</f>
-        <v>0</v>
+        <v>437</v>
       </c>
       <c r="V17" s="3">
         <f>S20</f>
-        <v>0</v>
+        <v>1418</v>
       </c>
       <c r="W17" s="3">
         <f>S21</f>
-        <v>0</v>
+        <v>911</v>
       </c>
       <c r="X17" s="3">
         <f>S22</f>
-        <v>0</v>
+        <v>1191</v>
       </c>
       <c r="Y17" s="3">
         <f>S23</f>
-        <v>0</v>
+        <v>1191</v>
       </c>
       <c r="Z17" s="3">
         <f>S24</f>
-        <v>0</v>
+        <v>1801</v>
       </c>
       <c r="AA17" s="3">
         <f>S25</f>
-        <v>0</v>
+        <v>1126</v>
       </c>
       <c r="AB17" s="3">
         <f>S26</f>
-        <v>0</v>
+        <v>842</v>
       </c>
       <c r="AC17" s="3">
         <f>S27</f>
-        <v>0</v>
+        <v>1680</v>
       </c>
       <c r="AD17" s="3">
         <f>S28</f>
-        <v>0</v>
+        <v>1871</v>
       </c>
       <c r="AE17" s="3">
         <f>S29</f>
-        <v>0</v>
+        <v>1807</v>
       </c>
       <c r="AF17" s="3">
         <f>S30</f>
-        <v>0</v>
+        <v>248</v>
       </c>
       <c r="AG17" s="3">
         <f>S31</f>
-        <v>0</v>
+        <v>1259</v>
       </c>
       <c r="AH17" s="3">
         <f>S32</f>
-        <v>0</v>
+        <v>555</v>
       </c>
       <c r="AI17" s="3">
         <f>S33</f>
-        <v>0</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="18" spans="1:35" x14ac:dyDescent="0.3">
@@ -2490,68 +2873,116 @@
       <c r="C18" t="s">
         <v>70</v>
       </c>
-      <c r="T18" s="4">
-        <v>0</v>
+      <c r="D18">
+        <v>2363</v>
+      </c>
+      <c r="E18">
+        <v>662</v>
+      </c>
+      <c r="F18">
+        <v>1095</v>
+      </c>
+      <c r="G18">
+        <v>1384</v>
+      </c>
+      <c r="H18">
+        <v>730</v>
+      </c>
+      <c r="I18">
+        <v>1380</v>
+      </c>
+      <c r="J18">
+        <v>1130</v>
+      </c>
+      <c r="K18">
+        <v>1243</v>
+      </c>
+      <c r="L18">
+        <v>1345</v>
+      </c>
+      <c r="M18">
+        <v>2068</v>
+      </c>
+      <c r="N18">
+        <v>1357</v>
+      </c>
+      <c r="O18">
+        <v>1591</v>
+      </c>
+      <c r="P18">
+        <v>1188</v>
+      </c>
+      <c r="Q18">
+        <v>1197</v>
+      </c>
+      <c r="R18">
+        <v>346</v>
+      </c>
+      <c r="S18">
+        <v>1464</v>
+      </c>
+      <c r="T18" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="U18" s="3">
         <f>T19</f>
-        <v>0</v>
+        <v>1776</v>
       </c>
       <c r="V18" s="3">
         <f>T20</f>
-        <v>0</v>
+        <v>1496</v>
       </c>
       <c r="W18" s="3">
         <f>T21</f>
-        <v>0</v>
+        <v>863</v>
       </c>
       <c r="X18" s="3">
         <f>T22</f>
-        <v>0</v>
+        <v>1283</v>
       </c>
       <c r="Y18" s="3">
         <f>T23</f>
-        <v>0</v>
+        <v>1283</v>
       </c>
       <c r="Z18" s="3">
         <f>T24</f>
-        <v>0</v>
+        <v>3128</v>
       </c>
       <c r="AA18" s="3">
         <f>T25</f>
-        <v>0</v>
+        <v>1192</v>
       </c>
       <c r="AB18" s="3">
         <f>T26</f>
-        <v>0</v>
+        <v>1178</v>
       </c>
       <c r="AC18" s="3">
         <f>T27</f>
-        <v>0</v>
+        <v>2657</v>
       </c>
       <c r="AD18" s="3">
         <f>T28</f>
-        <v>0</v>
+        <v>3333</v>
       </c>
       <c r="AE18" s="3">
         <f>T29</f>
-        <v>0</v>
+        <v>3139</v>
       </c>
       <c r="AF18" s="3">
         <f>T30</f>
-        <v>0</v>
+        <v>1215</v>
       </c>
       <c r="AG18" s="3">
         <f>T31</f>
-        <v>0</v>
+        <v>280</v>
       </c>
       <c r="AH18" s="3">
         <f>T32</f>
-        <v>0</v>
+        <v>910</v>
       </c>
       <c r="AI18" s="3">
         <f>T33</f>
-        <v>0</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="19" spans="1:35" x14ac:dyDescent="0.3">
@@ -2564,64 +2995,115 @@
       <c r="C19" t="s">
         <v>71</v>
       </c>
-      <c r="U19" s="4">
-        <v>0</v>
+      <c r="D19">
+        <v>1796</v>
+      </c>
+      <c r="E19">
+        <v>1114</v>
+      </c>
+      <c r="F19">
+        <v>1109</v>
+      </c>
+      <c r="G19">
+        <v>942</v>
+      </c>
+      <c r="H19">
+        <v>1165</v>
+      </c>
+      <c r="I19">
+        <v>410</v>
+      </c>
+      <c r="J19">
+        <v>703</v>
+      </c>
+      <c r="K19">
+        <v>753</v>
+      </c>
+      <c r="L19">
+        <v>991</v>
+      </c>
+      <c r="M19">
+        <v>914</v>
+      </c>
+      <c r="N19">
+        <v>694</v>
+      </c>
+      <c r="O19">
+        <v>279</v>
+      </c>
+      <c r="P19">
+        <v>1230</v>
+      </c>
+      <c r="Q19">
+        <v>592</v>
+      </c>
+      <c r="R19">
+        <v>1460</v>
+      </c>
+      <c r="S19">
+        <v>437</v>
+      </c>
+      <c r="T19">
+        <v>1776</v>
+      </c>
+      <c r="U19" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="V19" s="3">
         <f>U20</f>
-        <v>0</v>
+        <v>1407</v>
       </c>
       <c r="W19" s="3">
         <f>U21</f>
-        <v>0</v>
+        <v>1223</v>
       </c>
       <c r="X19" s="3">
         <f>U22</f>
-        <v>0</v>
+        <v>1206</v>
       </c>
       <c r="Y19" s="3">
         <f>U23</f>
-        <v>0</v>
+        <v>1206</v>
       </c>
       <c r="Z19" s="3">
         <f>U24</f>
-        <v>0</v>
+        <v>2039</v>
       </c>
       <c r="AA19" s="3">
         <f>U25</f>
-        <v>0</v>
+        <v>1176</v>
       </c>
       <c r="AB19" s="3">
         <f>U26</f>
-        <v>0</v>
+        <v>877</v>
       </c>
       <c r="AC19" s="3">
         <f>U27</f>
-        <v>0</v>
+        <v>1989</v>
       </c>
       <c r="AD19" s="3">
         <f>U28</f>
-        <v>0</v>
+        <v>1658</v>
       </c>
       <c r="AE19" s="3">
         <f>U29</f>
-        <v>0</v>
+        <v>2045</v>
       </c>
       <c r="AF19" s="3">
         <f>U30</f>
-        <v>0</v>
+        <v>560</v>
       </c>
       <c r="AG19" s="3">
         <f>U31</f>
-        <v>0</v>
+        <v>1570</v>
       </c>
       <c r="AH19" s="3">
         <f>U32</f>
-        <v>0</v>
+        <v>867</v>
       </c>
       <c r="AI19" s="3">
         <f>U33</f>
-        <v>0</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="20" spans="1:35" x14ac:dyDescent="0.3">
@@ -2634,60 +3116,114 @@
       <c r="C20" t="s">
         <v>70</v>
       </c>
-      <c r="V20" s="4">
-        <v>0</v>
+      <c r="D20">
+        <v>2686</v>
+      </c>
+      <c r="E20">
+        <v>1095</v>
+      </c>
+      <c r="F20">
+        <v>401</v>
+      </c>
+      <c r="G20">
+        <v>455</v>
+      </c>
+      <c r="H20">
+        <v>860</v>
+      </c>
+      <c r="I20">
+        <v>990</v>
+      </c>
+      <c r="J20">
+        <v>864</v>
+      </c>
+      <c r="K20">
+        <v>639</v>
+      </c>
+      <c r="L20">
+        <v>1761</v>
+      </c>
+      <c r="M20">
+        <v>1981</v>
+      </c>
+      <c r="N20">
+        <v>706</v>
+      </c>
+      <c r="O20">
+        <v>1197</v>
+      </c>
+      <c r="P20">
+        <v>1845</v>
+      </c>
+      <c r="Q20">
+        <v>936</v>
+      </c>
+      <c r="R20">
+        <v>1150</v>
+      </c>
+      <c r="S20">
+        <v>1418</v>
+      </c>
+      <c r="T20">
+        <v>1496</v>
+      </c>
+      <c r="U20">
+        <v>1407</v>
+      </c>
+      <c r="V20" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="W20" s="3">
         <f>V21</f>
-        <v>0</v>
+        <v>1518</v>
       </c>
       <c r="X20" s="3">
         <f>V22</f>
-        <v>0</v>
+        <v>215</v>
       </c>
       <c r="Y20" s="3">
         <f>V23</f>
-        <v>0</v>
+        <v>215</v>
       </c>
       <c r="Z20" s="3">
         <f>V24</f>
-        <v>0</v>
+        <v>3105</v>
       </c>
       <c r="AA20" s="3">
         <f>V25</f>
-        <v>0</v>
+        <v>305</v>
       </c>
       <c r="AB20" s="3">
         <f>V26</f>
-        <v>0</v>
+        <v>572</v>
       </c>
       <c r="AC20" s="3">
         <f>V27</f>
-        <v>0</v>
+        <v>3055</v>
       </c>
       <c r="AD20" s="3">
         <f>V28</f>
-        <v>0</v>
+        <v>3092</v>
       </c>
       <c r="AE20" s="3">
         <f>V29</f>
-        <v>0</v>
+        <v>3111</v>
       </c>
       <c r="AF20" s="3">
         <f>V30</f>
-        <v>0</v>
+        <v>1179</v>
       </c>
       <c r="AG20" s="3">
         <f>V31</f>
-        <v>0</v>
+        <v>1343</v>
       </c>
       <c r="AH20" s="3">
         <f>V32</f>
-        <v>0</v>
+        <v>1096</v>
       </c>
       <c r="AI20" s="3">
         <f>V33</f>
-        <v>0</v>
+        <v>435</v>
       </c>
     </row>
     <row r="21" spans="1:35" x14ac:dyDescent="0.3">
@@ -2700,56 +3236,113 @@
       <c r="C21" t="s">
         <v>69</v>
       </c>
-      <c r="W21" s="4">
-        <v>0</v>
+      <c r="D21">
+        <v>1523</v>
+      </c>
+      <c r="E21">
+        <v>469</v>
+      </c>
+      <c r="F21">
+        <v>1125</v>
+      </c>
+      <c r="G21">
+        <v>1237</v>
+      </c>
+      <c r="H21">
+        <v>713</v>
+      </c>
+      <c r="I21">
+        <v>925</v>
+      </c>
+      <c r="J21">
+        <v>811</v>
+      </c>
+      <c r="K21">
+        <v>1053</v>
+      </c>
+      <c r="L21">
+        <v>505</v>
+      </c>
+      <c r="M21">
+        <v>1383</v>
+      </c>
+      <c r="N21">
+        <v>1066</v>
+      </c>
+      <c r="O21">
+        <v>1130</v>
+      </c>
+      <c r="P21">
+        <v>348</v>
+      </c>
+      <c r="Q21">
+        <v>820</v>
+      </c>
+      <c r="R21">
+        <v>547</v>
+      </c>
+      <c r="S21">
+        <v>911</v>
+      </c>
+      <c r="T21">
+        <v>863</v>
+      </c>
+      <c r="U21">
+        <v>1223</v>
+      </c>
+      <c r="V21">
+        <v>1518</v>
+      </c>
+      <c r="W21" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="X21" s="3">
         <f>W22</f>
-        <v>0</v>
+        <v>1308</v>
       </c>
       <c r="Y21" s="3">
         <f>W23</f>
-        <v>0</v>
+        <v>1308</v>
       </c>
       <c r="Z21" s="3">
         <f>W24</f>
-        <v>0</v>
+        <v>2265</v>
       </c>
       <c r="AA21" s="3">
         <f>W25</f>
-        <v>0</v>
+        <v>1224</v>
       </c>
       <c r="AB21" s="3">
         <f>W26</f>
-        <v>0</v>
+        <v>1095</v>
       </c>
       <c r="AC21" s="3">
         <f>W27</f>
-        <v>0</v>
+        <v>1817</v>
       </c>
       <c r="AD21" s="3">
         <f>W28</f>
-        <v>0</v>
+        <v>2707</v>
       </c>
       <c r="AE21" s="3">
         <f>W29</f>
-        <v>0</v>
+        <v>2276</v>
       </c>
       <c r="AF21" s="3">
         <f>W30</f>
-        <v>0</v>
+        <v>677</v>
       </c>
       <c r="AG21" s="3">
         <f>W31</f>
-        <v>0</v>
+        <v>659</v>
       </c>
       <c r="AH21" s="3">
         <f>W32</f>
-        <v>0</v>
+        <v>533</v>
       </c>
       <c r="AI21" s="3">
         <f>W33</f>
-        <v>0</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="22" spans="1:35" x14ac:dyDescent="0.3">
@@ -2762,8 +3355,68 @@
       <c r="C22" t="s">
         <v>70</v>
       </c>
-      <c r="X22" s="4">
-        <v>0</v>
+      <c r="D22">
+        <v>2459</v>
+      </c>
+      <c r="E22">
+        <v>881</v>
+      </c>
+      <c r="F22">
+        <v>188</v>
+      </c>
+      <c r="G22">
+        <v>379</v>
+      </c>
+      <c r="H22">
+        <v>646</v>
+      </c>
+      <c r="I22">
+        <v>789</v>
+      </c>
+      <c r="J22">
+        <v>633</v>
+      </c>
+      <c r="K22">
+        <v>464</v>
+      </c>
+      <c r="L22">
+        <v>1546</v>
+      </c>
+      <c r="M22">
+        <v>1780</v>
+      </c>
+      <c r="N22">
+        <v>615</v>
+      </c>
+      <c r="O22">
+        <v>996</v>
+      </c>
+      <c r="P22">
+        <v>1631</v>
+      </c>
+      <c r="Q22">
+        <v>709</v>
+      </c>
+      <c r="R22">
+        <v>938</v>
+      </c>
+      <c r="S22">
+        <v>1191</v>
+      </c>
+      <c r="T22">
+        <v>1283</v>
+      </c>
+      <c r="U22">
+        <v>1206</v>
+      </c>
+      <c r="V22">
+        <v>215</v>
+      </c>
+      <c r="W22">
+        <v>1308</v>
+      </c>
+      <c r="X22" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="Y22" s="3">
         <f>X23</f>
@@ -2771,43 +3424,43 @@
       </c>
       <c r="Z22" s="3">
         <f>X24</f>
-        <v>0</v>
+        <v>2903</v>
       </c>
       <c r="AA22" s="3">
         <f>X25</f>
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="AB22" s="3">
         <f>X26</f>
-        <v>0</v>
+        <v>372</v>
       </c>
       <c r="AC22" s="3">
         <f>X27</f>
-        <v>0</v>
+        <v>2853</v>
       </c>
       <c r="AD22" s="3">
         <f>X28</f>
-        <v>0</v>
+        <v>2890</v>
       </c>
       <c r="AE22" s="3">
         <f>X29</f>
-        <v>0</v>
+        <v>2909</v>
       </c>
       <c r="AF22" s="3">
         <f>X30</f>
-        <v>0</v>
+        <v>953</v>
       </c>
       <c r="AG22" s="3">
         <f>X31</f>
-        <v>0</v>
+        <v>1133</v>
       </c>
       <c r="AH22" s="3">
         <f>X32</f>
-        <v>0</v>
+        <v>886</v>
       </c>
       <c r="AI22" s="3">
         <f>X33</f>
-        <v>0</v>
+        <v>225</v>
       </c>
     </row>
     <row r="23" spans="1:35" x14ac:dyDescent="0.3">
@@ -2820,48 +3473,111 @@
       <c r="C23" t="s">
         <v>70</v>
       </c>
-      <c r="Y23" s="4">
+      <c r="D23">
+        <v>2459</v>
+      </c>
+      <c r="E23">
+        <v>881</v>
+      </c>
+      <c r="F23">
+        <v>188</v>
+      </c>
+      <c r="G23">
+        <v>379</v>
+      </c>
+      <c r="H23">
+        <v>646</v>
+      </c>
+      <c r="I23">
+        <v>789</v>
+      </c>
+      <c r="J23">
+        <v>633</v>
+      </c>
+      <c r="K23">
+        <v>464</v>
+      </c>
+      <c r="L23">
+        <v>1546</v>
+      </c>
+      <c r="M23">
+        <v>1780</v>
+      </c>
+      <c r="N23">
+        <v>615</v>
+      </c>
+      <c r="O23">
+        <v>996</v>
+      </c>
+      <c r="P23">
+        <v>1631</v>
+      </c>
+      <c r="Q23">
+        <v>709</v>
+      </c>
+      <c r="R23">
+        <v>938</v>
+      </c>
+      <c r="S23">
+        <v>1191</v>
+      </c>
+      <c r="T23">
+        <v>1283</v>
+      </c>
+      <c r="U23">
+        <v>1206</v>
+      </c>
+      <c r="V23">
+        <v>215</v>
+      </c>
+      <c r="W23">
+        <v>1308</v>
+      </c>
+      <c r="X23">
         <v>0</v>
+      </c>
+      <c r="Y23" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="Z23" s="3">
         <f>Y24</f>
-        <v>0</v>
+        <v>2903</v>
       </c>
       <c r="AA23" s="3">
         <f>Y25</f>
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="AB23" s="3">
         <f>Y26</f>
-        <v>0</v>
+        <v>372</v>
       </c>
       <c r="AC23" s="3">
         <f>Y27</f>
-        <v>0</v>
+        <v>2853</v>
       </c>
       <c r="AD23" s="3">
         <f>Y28</f>
-        <v>0</v>
+        <v>2890</v>
       </c>
       <c r="AE23" s="3">
         <f>Y29</f>
-        <v>0</v>
+        <v>2909</v>
       </c>
       <c r="AF23" s="3">
         <f>Y30</f>
-        <v>0</v>
+        <v>953</v>
       </c>
       <c r="AG23" s="3">
         <f>Y31</f>
-        <v>0</v>
+        <v>1133</v>
       </c>
       <c r="AH23" s="3">
         <f>Y32</f>
-        <v>0</v>
+        <v>886</v>
       </c>
       <c r="AI23" s="3">
         <f>Y33</f>
-        <v>0</v>
+        <v>225</v>
       </c>
     </row>
     <row r="24" spans="1:35" x14ac:dyDescent="0.3">
@@ -2874,44 +3590,110 @@
       <c r="C24" t="s">
         <v>68</v>
       </c>
-      <c r="Z24" s="4">
-        <v>0</v>
+      <c r="D24">
+        <v>742</v>
+      </c>
+      <c r="E24">
+        <v>2466</v>
+      </c>
+      <c r="F24">
+        <v>2813</v>
+      </c>
+      <c r="G24">
+        <v>2646</v>
+      </c>
+      <c r="H24">
+        <v>2762</v>
+      </c>
+      <c r="I24">
+        <v>2129</v>
+      </c>
+      <c r="J24">
+        <v>2382</v>
+      </c>
+      <c r="K24">
+        <v>2457</v>
+      </c>
+      <c r="L24">
+        <v>1824</v>
+      </c>
+      <c r="M24">
+        <v>1263</v>
+      </c>
+      <c r="N24">
+        <v>2394</v>
+      </c>
+      <c r="O24">
+        <v>2227</v>
+      </c>
+      <c r="P24">
+        <v>1918</v>
+      </c>
+      <c r="Q24">
+        <v>2268</v>
+      </c>
+      <c r="R24">
+        <v>2812</v>
+      </c>
+      <c r="S24">
+        <v>1801</v>
+      </c>
+      <c r="T24">
+        <v>3128</v>
+      </c>
+      <c r="U24">
+        <v>2039</v>
+      </c>
+      <c r="V24">
+        <v>3105</v>
+      </c>
+      <c r="W24">
+        <v>2265</v>
+      </c>
+      <c r="X24">
+        <v>2903</v>
+      </c>
+      <c r="Y24">
+        <v>2903</v>
+      </c>
+      <c r="Z24" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="AA24" s="3">
         <f>Z25</f>
-        <v>0</v>
+        <v>2870</v>
       </c>
       <c r="AB24" s="3">
         <f>Z26</f>
-        <v>0</v>
+        <v>2571</v>
       </c>
       <c r="AC24" s="3">
         <f>Z27</f>
-        <v>0</v>
+        <v>496</v>
       </c>
       <c r="AD24" s="3">
         <f>Z28</f>
-        <v>0</v>
+        <v>803</v>
       </c>
       <c r="AE24" s="3">
         <f>Z29</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AF24" s="3">
         <f>Z30</f>
-        <v>0</v>
+        <v>2050</v>
       </c>
       <c r="AG24" s="3">
         <f>Z31</f>
-        <v>0</v>
+        <v>2924</v>
       </c>
       <c r="AH24" s="3">
         <f>Z32</f>
-        <v>0</v>
+        <v>2293</v>
       </c>
       <c r="AI24" s="3">
         <f>Z33</f>
-        <v>0</v>
+        <v>2807</v>
       </c>
     </row>
     <row r="25" spans="1:35" x14ac:dyDescent="0.3">
@@ -2924,40 +3706,109 @@
       <c r="C25" t="s">
         <v>70</v>
       </c>
-      <c r="AA25" s="4">
-        <v>0</v>
+      <c r="D25">
+        <v>2394</v>
+      </c>
+      <c r="E25">
+        <v>774</v>
+      </c>
+      <c r="F25">
+        <v>97</v>
+      </c>
+      <c r="G25">
+        <v>381</v>
+      </c>
+      <c r="H25">
+        <v>533</v>
+      </c>
+      <c r="I25">
+        <v>758</v>
+      </c>
+      <c r="J25">
+        <v>568</v>
+      </c>
+      <c r="K25">
+        <v>433</v>
+      </c>
+      <c r="L25">
+        <v>1462</v>
+      </c>
+      <c r="M25">
+        <v>1729</v>
+      </c>
+      <c r="N25">
+        <v>584</v>
+      </c>
+      <c r="O25">
+        <v>965</v>
+      </c>
+      <c r="P25">
+        <v>1547</v>
+      </c>
+      <c r="Q25">
+        <v>644</v>
+      </c>
+      <c r="R25">
+        <v>847</v>
+      </c>
+      <c r="S25">
+        <v>1126</v>
+      </c>
+      <c r="T25">
+        <v>1192</v>
+      </c>
+      <c r="U25">
+        <v>1176</v>
+      </c>
+      <c r="V25">
+        <v>305</v>
+      </c>
+      <c r="W25">
+        <v>1224</v>
+      </c>
+      <c r="X25">
+        <v>95</v>
+      </c>
+      <c r="Y25">
+        <v>95</v>
+      </c>
+      <c r="Z25">
+        <v>2870</v>
+      </c>
+      <c r="AA25" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="AB25" s="3">
         <f>AA26</f>
-        <v>0</v>
+        <v>305</v>
       </c>
       <c r="AC25" s="3">
         <f>AA27</f>
-        <v>0</v>
+        <v>2737</v>
       </c>
       <c r="AD25" s="3">
         <f>AA28</f>
-        <v>0</v>
+        <v>2859</v>
       </c>
       <c r="AE25" s="3">
         <f>AA29</f>
-        <v>0</v>
+        <v>2878</v>
       </c>
       <c r="AF25" s="3">
         <f>AA30</f>
-        <v>0</v>
+        <v>886</v>
       </c>
       <c r="AG25" s="3">
         <f>AA31</f>
-        <v>0</v>
+        <v>1044</v>
       </c>
       <c r="AH25" s="3">
         <f>AA32</f>
-        <v>0</v>
+        <v>824</v>
       </c>
       <c r="AI25" s="3">
         <f>AA33</f>
-        <v>0</v>
+        <v>136</v>
       </c>
     </row>
     <row r="26" spans="1:35" x14ac:dyDescent="0.3">
@@ -2970,36 +3821,108 @@
       <c r="C26" t="s">
         <v>71</v>
       </c>
-      <c r="AB26" s="4">
-        <v>0</v>
+      <c r="D26">
+        <v>2110</v>
+      </c>
+      <c r="E26">
+        <v>685</v>
+      </c>
+      <c r="F26">
+        <v>246</v>
+      </c>
+      <c r="G26">
+        <v>215</v>
+      </c>
+      <c r="H26">
+        <v>450</v>
+      </c>
+      <c r="I26">
+        <v>460</v>
+      </c>
+      <c r="J26">
+        <v>284</v>
+      </c>
+      <c r="K26">
+        <v>134</v>
+      </c>
+      <c r="L26">
+        <v>1220</v>
+      </c>
+      <c r="M26">
+        <v>1445</v>
+      </c>
+      <c r="N26">
+        <v>285</v>
+      </c>
+      <c r="O26">
+        <v>666</v>
+      </c>
+      <c r="P26">
+        <v>1418</v>
+      </c>
+      <c r="Q26">
+        <v>360</v>
+      </c>
+      <c r="R26">
+        <v>831</v>
+      </c>
+      <c r="S26">
+        <v>842</v>
+      </c>
+      <c r="T26">
+        <v>1178</v>
+      </c>
+      <c r="U26">
+        <v>877</v>
+      </c>
+      <c r="V26">
+        <v>572</v>
+      </c>
+      <c r="W26">
+        <v>1095</v>
+      </c>
+      <c r="X26">
+        <v>372</v>
+      </c>
+      <c r="Y26">
+        <v>372</v>
+      </c>
+      <c r="Z26">
+        <v>2571</v>
+      </c>
+      <c r="AA26">
+        <v>305</v>
+      </c>
+      <c r="AB26" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="AC26" s="3">
         <f>AB27</f>
-        <v>0</v>
+        <v>2453</v>
       </c>
       <c r="AD26" s="3">
         <f>AB28</f>
-        <v>0</v>
+        <v>2560</v>
       </c>
       <c r="AE26" s="3">
         <f>AB29</f>
-        <v>0</v>
+        <v>2579</v>
       </c>
       <c r="AF26" s="3">
         <f>AB30</f>
-        <v>0</v>
+        <v>602</v>
       </c>
       <c r="AG26" s="3">
         <f>AB31</f>
-        <v>0</v>
+        <v>1027</v>
       </c>
       <c r="AH26" s="3">
         <f>AB32</f>
-        <v>0</v>
+        <v>561</v>
       </c>
       <c r="AI26" s="3">
         <f>AB33</f>
-        <v>0</v>
+        <v>243</v>
       </c>
     </row>
     <row r="27" spans="1:35" x14ac:dyDescent="0.3">
@@ -3015,32 +3938,104 @@
       <c r="D27">
         <v>355</v>
       </c>
-      <c r="AC27" s="4">
-        <v>0</v>
+      <c r="E27">
+        <v>2141</v>
+      </c>
+      <c r="F27">
+        <v>2667</v>
+      </c>
+      <c r="G27">
+        <v>2597</v>
+      </c>
+      <c r="H27">
+        <v>2387</v>
+      </c>
+      <c r="I27">
+        <v>2079</v>
+      </c>
+      <c r="J27">
+        <v>2202</v>
+      </c>
+      <c r="K27">
+        <v>2408</v>
+      </c>
+      <c r="L27">
+        <v>1360</v>
+      </c>
+      <c r="M27">
+        <v>1079</v>
+      </c>
+      <c r="N27">
+        <v>2344</v>
+      </c>
+      <c r="O27">
+        <v>2178</v>
+      </c>
+      <c r="P27">
+        <v>1472</v>
+      </c>
+      <c r="Q27">
+        <v>2093</v>
+      </c>
+      <c r="R27">
+        <v>2341</v>
+      </c>
+      <c r="S27">
+        <v>1680</v>
+      </c>
+      <c r="T27">
+        <v>2657</v>
+      </c>
+      <c r="U27">
+        <v>1989</v>
+      </c>
+      <c r="V27">
+        <v>3055</v>
+      </c>
+      <c r="W27">
+        <v>1817</v>
+      </c>
+      <c r="X27">
+        <v>2853</v>
+      </c>
+      <c r="Y27">
+        <v>2853</v>
+      </c>
+      <c r="Z27">
+        <v>496</v>
+      </c>
+      <c r="AA27">
+        <v>2737</v>
+      </c>
+      <c r="AB27">
+        <v>2453</v>
+      </c>
+      <c r="AC27" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="AD27" s="3">
         <f>AC28</f>
-        <v>0</v>
+        <v>1257</v>
       </c>
       <c r="AE27" s="3">
         <f>AC29</f>
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="AF27" s="3">
         <f>AC30</f>
-        <v>0</v>
+        <v>1852</v>
       </c>
       <c r="AG27" s="3">
         <f>AC31</f>
-        <v>0</v>
+        <v>2452</v>
       </c>
       <c r="AH27" s="3">
         <f>AC32</f>
-        <v>0</v>
+        <v>2025</v>
       </c>
       <c r="AI27" s="3">
         <f>AC33</f>
-        <v>0</v>
+        <v>2691</v>
       </c>
     </row>
     <row r="28" spans="1:35" x14ac:dyDescent="0.3">
@@ -3053,28 +4048,106 @@
       <c r="C28" t="s">
         <v>68</v>
       </c>
-      <c r="AD28" s="4">
-        <v>0</v>
+      <c r="D28">
+        <v>1508</v>
+      </c>
+      <c r="E28">
+        <v>2670</v>
+      </c>
+      <c r="F28">
+        <v>2800</v>
+      </c>
+      <c r="G28">
+        <v>2633</v>
+      </c>
+      <c r="H28">
+        <v>2831</v>
+      </c>
+      <c r="I28">
+        <v>2101</v>
+      </c>
+      <c r="J28">
+        <v>2388</v>
+      </c>
+      <c r="K28">
+        <v>2444</v>
+      </c>
+      <c r="L28">
+        <v>2204</v>
+      </c>
+      <c r="M28">
+        <v>1332</v>
+      </c>
+      <c r="N28">
+        <v>2386</v>
+      </c>
+      <c r="O28">
+        <v>1937</v>
+      </c>
+      <c r="P28">
+        <v>2443</v>
+      </c>
+      <c r="Q28">
+        <v>2273</v>
+      </c>
+      <c r="R28">
+        <v>3016</v>
+      </c>
+      <c r="S28">
+        <v>1871</v>
+      </c>
+      <c r="T28">
+        <v>3333</v>
+      </c>
+      <c r="U28">
+        <v>1658</v>
+      </c>
+      <c r="V28">
+        <v>3092</v>
+      </c>
+      <c r="W28">
+        <v>2707</v>
+      </c>
+      <c r="X28">
+        <v>2890</v>
+      </c>
+      <c r="Y28">
+        <v>2890</v>
+      </c>
+      <c r="Z28">
+        <v>803</v>
+      </c>
+      <c r="AA28">
+        <v>2859</v>
+      </c>
+      <c r="AB28">
+        <v>2560</v>
+      </c>
+      <c r="AC28">
+        <v>1257</v>
+      </c>
+      <c r="AD28" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="AE28" s="3">
         <f>AD29</f>
-        <v>0</v>
+        <v>809</v>
       </c>
       <c r="AF28" s="3">
         <f>AD30</f>
-        <v>0</v>
+        <v>2145</v>
       </c>
       <c r="AG28" s="3">
         <f>AD31</f>
-        <v>0</v>
+        <v>3155</v>
       </c>
       <c r="AH28" s="3">
         <f>AD32</f>
-        <v>0</v>
+        <v>2451</v>
       </c>
       <c r="AI28" s="3">
         <f>AD33</f>
-        <v>0</v>
+        <v>2805</v>
       </c>
     </row>
     <row r="29" spans="1:35" x14ac:dyDescent="0.3">
@@ -3087,24 +4160,105 @@
       <c r="C29" t="s">
         <v>68</v>
       </c>
-      <c r="AE29" s="4">
-        <v>0</v>
+      <c r="D29">
+        <v>754</v>
+      </c>
+      <c r="E29">
+        <v>2477</v>
+      </c>
+      <c r="F29">
+        <v>2819</v>
+      </c>
+      <c r="G29">
+        <v>2652</v>
+      </c>
+      <c r="H29">
+        <v>2768</v>
+      </c>
+      <c r="I29">
+        <v>2135</v>
+      </c>
+      <c r="J29">
+        <v>2388</v>
+      </c>
+      <c r="K29">
+        <v>2463</v>
+      </c>
+      <c r="L29">
+        <v>1835</v>
+      </c>
+      <c r="M29">
+        <v>1269</v>
+      </c>
+      <c r="N29">
+        <v>2400</v>
+      </c>
+      <c r="O29">
+        <v>2233</v>
+      </c>
+      <c r="P29">
+        <v>1930</v>
+      </c>
+      <c r="Q29">
+        <v>2274</v>
+      </c>
+      <c r="R29">
+        <v>2823</v>
+      </c>
+      <c r="S29">
+        <v>1807</v>
+      </c>
+      <c r="T29">
+        <v>3139</v>
+      </c>
+      <c r="U29">
+        <v>2045</v>
+      </c>
+      <c r="V29">
+        <v>3111</v>
+      </c>
+      <c r="W29">
+        <v>2276</v>
+      </c>
+      <c r="X29">
+        <v>2909</v>
+      </c>
+      <c r="Y29">
+        <v>2909</v>
+      </c>
+      <c r="Z29">
+        <v>12</v>
+      </c>
+      <c r="AA29">
+        <v>2878</v>
+      </c>
+      <c r="AB29">
+        <v>2579</v>
+      </c>
+      <c r="AC29">
+        <v>503</v>
+      </c>
+      <c r="AD29">
+        <v>809</v>
+      </c>
+      <c r="AE29" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="AF29" s="3">
         <f>AE30</f>
-        <v>0</v>
+        <v>2055</v>
       </c>
       <c r="AG29" s="3">
         <f>AE31</f>
-        <v>0</v>
+        <v>2935</v>
       </c>
       <c r="AH29" s="3">
         <f>AE32</f>
-        <v>0</v>
+        <v>2361</v>
       </c>
       <c r="AI29" s="3">
         <f>AE33</f>
-        <v>0</v>
+        <v>2813</v>
       </c>
     </row>
     <row r="30" spans="1:35" x14ac:dyDescent="0.3">
@@ -3117,20 +4271,104 @@
       <c r="C30" t="s">
         <v>68</v>
       </c>
-      <c r="AF30" s="4">
-        <v>0</v>
+      <c r="D30">
+        <v>1509</v>
+      </c>
+      <c r="E30">
+        <v>553</v>
+      </c>
+      <c r="F30">
+        <v>816</v>
+      </c>
+      <c r="G30">
+        <v>742</v>
+      </c>
+      <c r="H30">
+        <v>714</v>
+      </c>
+      <c r="I30">
+        <v>294</v>
+      </c>
+      <c r="J30">
+        <v>351</v>
+      </c>
+      <c r="K30">
+        <v>559</v>
+      </c>
+      <c r="L30">
+        <v>652</v>
+      </c>
+      <c r="M30">
+        <v>851</v>
+      </c>
+      <c r="N30">
+        <v>525</v>
+      </c>
+      <c r="O30">
+        <v>487</v>
+      </c>
+      <c r="P30">
+        <v>851</v>
+      </c>
+      <c r="Q30">
+        <v>242</v>
+      </c>
+      <c r="R30">
+        <v>899</v>
+      </c>
+      <c r="S30">
+        <v>248</v>
+      </c>
+      <c r="T30">
+        <v>1215</v>
+      </c>
+      <c r="U30">
+        <v>560</v>
+      </c>
+      <c r="V30">
+        <v>1179</v>
+      </c>
+      <c r="W30">
+        <v>677</v>
+      </c>
+      <c r="X30">
+        <v>953</v>
+      </c>
+      <c r="Y30">
+        <v>953</v>
+      </c>
+      <c r="Z30">
+        <v>2050</v>
+      </c>
+      <c r="AA30">
+        <v>886</v>
+      </c>
+      <c r="AB30">
+        <v>602</v>
+      </c>
+      <c r="AC30">
+        <v>1852</v>
+      </c>
+      <c r="AD30">
+        <v>2145</v>
+      </c>
+      <c r="AE30">
+        <v>2055</v>
+      </c>
+      <c r="AF30" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="AG30" s="3">
         <f>AF31</f>
-        <v>0</v>
+        <v>1012</v>
       </c>
       <c r="AH30" s="3">
         <f>AF32</f>
-        <v>0</v>
+        <v>308</v>
       </c>
       <c r="AI30" s="3">
         <f>AF33</f>
-        <v>0</v>
+        <v>825</v>
       </c>
     </row>
     <row r="31" spans="1:35" x14ac:dyDescent="0.3">
@@ -3143,16 +4381,103 @@
       <c r="C31" t="s">
         <v>69</v>
       </c>
-      <c r="AG31" s="4">
-        <v>0</v>
+      <c r="D31">
+        <v>2158</v>
+      </c>
+      <c r="E31">
+        <v>457</v>
+      </c>
+      <c r="F31">
+        <v>947</v>
+      </c>
+      <c r="G31">
+        <v>1235</v>
+      </c>
+      <c r="H31">
+        <v>581</v>
+      </c>
+      <c r="I31">
+        <v>1175</v>
+      </c>
+      <c r="J31">
+        <v>925</v>
+      </c>
+      <c r="K31">
+        <v>1095</v>
+      </c>
+      <c r="L31">
+        <v>1140</v>
+      </c>
+      <c r="M31">
+        <v>1861</v>
+      </c>
+      <c r="N31">
+        <v>1179</v>
+      </c>
+      <c r="O31">
+        <v>1386</v>
+      </c>
+      <c r="P31">
+        <v>983</v>
+      </c>
+      <c r="Q31">
+        <v>992</v>
+      </c>
+      <c r="R31">
+        <v>200</v>
+      </c>
+      <c r="S31">
+        <v>1259</v>
+      </c>
+      <c r="T31">
+        <v>280</v>
+      </c>
+      <c r="U31">
+        <v>1570</v>
+      </c>
+      <c r="V31">
+        <v>1343</v>
+      </c>
+      <c r="W31">
+        <v>659</v>
+      </c>
+      <c r="X31">
+        <v>1133</v>
+      </c>
+      <c r="Y31">
+        <v>1133</v>
+      </c>
+      <c r="Z31">
+        <v>2924</v>
+      </c>
+      <c r="AA31">
+        <v>1044</v>
+      </c>
+      <c r="AB31">
+        <v>1027</v>
+      </c>
+      <c r="AC31">
+        <v>2452</v>
+      </c>
+      <c r="AD31">
+        <v>3155</v>
+      </c>
+      <c r="AE31">
+        <v>2935</v>
+      </c>
+      <c r="AF31">
+        <v>1012</v>
+      </c>
+      <c r="AG31" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="AH31" s="3">
         <f>AG32</f>
-        <v>0</v>
+        <v>704</v>
       </c>
       <c r="AI31" s="3">
         <f>AG33</f>
-        <v>0</v>
+        <v>908</v>
       </c>
     </row>
     <row r="32" spans="1:35" x14ac:dyDescent="0.3">
@@ -3165,12 +4490,102 @@
       <c r="C32" t="s">
         <v>69</v>
       </c>
-      <c r="AH32" s="4">
-        <v>0</v>
+      <c r="D32">
+        <v>1682</v>
+      </c>
+      <c r="E32">
+        <v>248</v>
+      </c>
+      <c r="F32">
+        <v>704</v>
+      </c>
+      <c r="G32">
+        <v>705</v>
+      </c>
+      <c r="H32">
+        <v>408</v>
+      </c>
+      <c r="I32">
+        <v>471</v>
+      </c>
+      <c r="J32">
+        <v>279</v>
+      </c>
+      <c r="K32">
+        <v>521</v>
+      </c>
+      <c r="L32">
+        <v>661</v>
+      </c>
+      <c r="M32">
+        <v>1158</v>
+      </c>
+      <c r="N32">
+        <v>534</v>
+      </c>
+      <c r="O32">
+        <v>681</v>
+      </c>
+      <c r="P32">
+        <v>857</v>
+      </c>
+      <c r="Q32">
+        <v>287</v>
+      </c>
+      <c r="R32">
+        <v>593</v>
+      </c>
+      <c r="S32">
+        <v>555</v>
+      </c>
+      <c r="T32">
+        <v>910</v>
+      </c>
+      <c r="U32">
+        <v>867</v>
+      </c>
+      <c r="V32">
+        <v>1096</v>
+      </c>
+      <c r="W32">
+        <v>533</v>
+      </c>
+      <c r="X32">
+        <v>886</v>
+      </c>
+      <c r="Y32">
+        <v>886</v>
+      </c>
+      <c r="Z32">
+        <v>2293</v>
+      </c>
+      <c r="AA32">
+        <v>824</v>
+      </c>
+      <c r="AB32">
+        <v>561</v>
+      </c>
+      <c r="AC32">
+        <v>2025</v>
+      </c>
+      <c r="AD32">
+        <v>2451</v>
+      </c>
+      <c r="AE32">
+        <v>2361</v>
+      </c>
+      <c r="AF32">
+        <v>308</v>
+      </c>
+      <c r="AG32">
+        <v>704</v>
+      </c>
+      <c r="AH32" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="AI32" s="3">
         <f>AH33</f>
-        <v>0</v>
+        <v>666</v>
       </c>
     </row>
     <row r="33" spans="1:35" x14ac:dyDescent="0.3">
@@ -3183,54 +4598,177 @@
       <c r="C33" t="s">
         <v>70</v>
       </c>
-      <c r="AI33" s="4">
-        <v>0</v>
+      <c r="D33">
+        <v>2348</v>
+      </c>
+      <c r="E33">
+        <v>638</v>
+      </c>
+      <c r="F33">
+        <v>39</v>
+      </c>
+      <c r="G33">
+        <v>382</v>
+      </c>
+      <c r="H33">
+        <v>397</v>
+      </c>
+      <c r="I33">
+        <v>696</v>
+      </c>
+      <c r="J33">
+        <v>506</v>
+      </c>
+      <c r="K33">
+        <v>371</v>
+      </c>
+      <c r="L33">
+        <v>1327</v>
+      </c>
+      <c r="M33">
+        <v>1667</v>
+      </c>
+      <c r="N33">
+        <v>522</v>
+      </c>
+      <c r="O33">
+        <v>903</v>
+      </c>
+      <c r="P33">
+        <v>1412</v>
+      </c>
+      <c r="Q33">
+        <v>582</v>
+      </c>
+      <c r="R33">
+        <v>711</v>
+      </c>
+      <c r="S33">
+        <v>1064</v>
+      </c>
+      <c r="T33">
+        <v>1056</v>
+      </c>
+      <c r="U33">
+        <v>1113</v>
+      </c>
+      <c r="V33">
+        <v>435</v>
+      </c>
+      <c r="W33">
+        <v>1089</v>
+      </c>
+      <c r="X33">
+        <v>225</v>
+      </c>
+      <c r="Y33">
+        <v>225</v>
+      </c>
+      <c r="Z33">
+        <v>2807</v>
+      </c>
+      <c r="AA33">
+        <v>136</v>
+      </c>
+      <c r="AB33">
+        <v>243</v>
+      </c>
+      <c r="AC33">
+        <v>2691</v>
+      </c>
+      <c r="AD33">
+        <v>2805</v>
+      </c>
+      <c r="AE33">
+        <v>2813</v>
+      </c>
+      <c r="AF33">
+        <v>825</v>
+      </c>
+      <c r="AG33">
+        <v>908</v>
+      </c>
+      <c r="AH33">
+        <v>666</v>
+      </c>
+      <c r="AI33" s="7" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="34" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A34" s="5"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
-      <c r="I34" s="5"/>
-      <c r="J34" s="5"/>
-      <c r="K34" s="5"/>
-      <c r="L34" s="5"/>
-      <c r="M34" s="5"/>
-      <c r="N34" s="5"/>
-      <c r="O34" s="5"/>
-      <c r="P34" s="5"/>
-      <c r="Q34" s="5"/>
-      <c r="R34" s="5"/>
-      <c r="S34" s="5"/>
-      <c r="T34" s="5"/>
-      <c r="U34" s="5"/>
-      <c r="V34" s="5"/>
-      <c r="W34" s="5"/>
-      <c r="X34" s="5"/>
-      <c r="Y34" s="5"/>
-      <c r="Z34" s="5"/>
-      <c r="AA34" s="5"/>
-      <c r="AB34" s="5"/>
-      <c r="AC34" s="5"/>
-      <c r="AD34" s="5"/>
-      <c r="AE34" s="5"/>
-      <c r="AF34" s="5"/>
-      <c r="AG34" s="5"/>
-      <c r="AH34" s="5"/>
-      <c r="AI34" s="5"/>
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+      <c r="K34" s="4"/>
+      <c r="L34" s="4"/>
+      <c r="M34" s="4"/>
+      <c r="N34" s="4"/>
+      <c r="O34" s="4"/>
+      <c r="P34" s="4"/>
+      <c r="Q34" s="4"/>
+      <c r="R34" s="4"/>
+      <c r="S34" s="4"/>
+      <c r="T34" s="4"/>
+      <c r="U34" s="4"/>
+      <c r="V34" s="4"/>
+      <c r="W34" s="4"/>
+      <c r="X34" s="4"/>
+      <c r="Y34" s="4"/>
+      <c r="Z34" s="4"/>
+      <c r="AA34" s="4"/>
+      <c r="AB34" s="4"/>
+      <c r="AC34" s="4"/>
+      <c r="AD34" s="4"/>
+      <c r="AE34" s="4"/>
+      <c r="AF34" s="4"/>
+      <c r="AG34" s="4"/>
+      <c r="AH34" s="4"/>
+      <c r="AI34" s="4"/>
     </row>
     <row r="36" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>73</v>
+      <c r="B36" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="38" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>75</v>
+      </c>
+      <c r="C38" s="8">
+        <f>AVERAGE($D$2:$AI$33)</f>
+        <v>1234.0241935483871</v>
+      </c>
+    </row>
+    <row r="39" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>76</v>
+      </c>
+      <c r="C39" s="8">
+        <f>MEDIAN($D$2:$AI$33)</f>
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="40" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>77</v>
+      </c>
+      <c r="C40" s="8">
+        <f>MODE($D$2:$AI$33)</f>
+        <v>1095</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B36" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>